<commit_message>
half of datas of farmandehi added
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammad/Library/CloudStorage/OneDrive-email.kntu.ac.ir/MangerDashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061A1BBA-DD43-B34F-998D-5DA070BE8F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76FA512-2616-E341-B19B-F7BD79FF46B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{490754A7-E054-EF47-883C-C68C37A7F559}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{490754A7-E054-EF47-883C-C68C37A7F559}"/>
   </bookViews>
   <sheets>
     <sheet name="صفحه اصلی" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="شاخص‌های عمومی" sheetId="7" r:id="rId3"/>
     <sheet name="شاخص‌های مدیریتی و فرماندهی" sheetId="14" r:id="rId4"/>
     <sheet name="دیتا عمومی" sheetId="11" r:id="rId5"/>
-    <sheet name="نمودارها" sheetId="8" r:id="rId6"/>
-    <sheet name="ماه‌ها" sheetId="10" state="hidden" r:id="rId7"/>
+    <sheet name="دیتا مدیرتی و فرماندهی" sheetId="15" r:id="rId6"/>
+    <sheet name="نمودارها" sheetId="8" r:id="rId7"/>
+    <sheet name="ماه‌ها" sheetId="10" state="hidden" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'صفحه اصلی'!$A$1:$I$28</definedName>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="247">
   <si>
     <t>نام و نام خانوادگی</t>
   </si>
@@ -12467,7 +12468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9425791-3090-8148-9A7C-2897ADB7D5A1}">
   <dimension ref="A1:DO35"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -13013,7 +13014,7 @@
         <f t="shared" si="9"/>
         <v>مدیریتی ۸</v>
       </c>
-      <c r="CW2" s="38" t="str">
+      <c r="CW2" s="21" t="str">
         <f t="shared" si="9"/>
         <v>مدیریتی ۹</v>
       </c>
@@ -22534,6 +22535,847 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10993374-1CDE-D345-894E-3CB87C699537}">
+  <dimension ref="A1:DD4"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="BC2" sqref="BC2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="X1" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y1" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB1" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC1" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD1" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AE1" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="AF1" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="AG1" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="AH1" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="AI1" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="AJ1" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="AK1" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="AL1" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="AM1" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="AN1" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="AO1" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="AP1" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="AQ1" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="AR1" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="AS1" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="AT1" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="AU1" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="AV1" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="AW1" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="AX1" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="AY1" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="AZ1" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="BA1" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="BB1" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="BC1" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="BD1" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="BE1" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="BF1" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="BG1" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="BH1" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="BI1" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="BJ1" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="BK1" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="BL1" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="BM1" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="BN1" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="BO1" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="BP1" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="BQ1" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="BR1" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="BS1" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="BT1" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="BU1" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="BV1" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="BW1" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="BX1" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="BY1" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="BZ1" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="CA1" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="CB1" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="CC1" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="CD1" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="CE1" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="CF1" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="CG1" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="CH1" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="CI1" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="CJ1" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="CK1" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="CL1" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="CM1" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="CN1" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="CO1" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="CP1" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="CQ1" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="CR1" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="CS1" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="CT1" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="CU1" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="CV1" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="CW1" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="CX1" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="CY1" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="CZ1" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="DA1" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="DB1" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="DC1" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="DD1" s="13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:108" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" cm="1">
+        <f t="array" ref="A2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!C3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!C4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!C5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!C6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!C7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!C8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!C9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!C10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!C11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!C12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!C13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!C14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!C15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!C16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!C17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!C18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!C19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!C20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!C21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!C22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!C23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!C24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!C25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!C26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!C27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!C28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!C29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!C30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!C31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!C32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!C33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!C3)</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" cm="1">
+        <f t="array" ref="B2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!D3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!D4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!D5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!D6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!D7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!D8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!D9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!D10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!D11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!D12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!D13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!D14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!D15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!D16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!D17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!D18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!D19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!D20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!D21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!D22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!D23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!D24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!D25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!D26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!D27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!D28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!D29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!D30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!D31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!D32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!D33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!D3)</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="11" cm="1">
+        <f t="array" ref="C2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!E3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!E4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!E5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!E6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!E7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!E8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!E9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!E10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!E11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!E12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!E13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!E14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!E15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!E16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!E17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!E18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!E19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!E20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!E21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!E22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!E23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!E24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!E25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!E26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!E27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!E28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!E29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!E30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!E31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!E32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!E33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!E3)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" cm="1">
+        <f t="array" ref="D2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!F3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!F4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!F5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!F6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!F7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!F8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!F9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!F10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!F11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!F12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!F13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!F14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!F15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!F16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!F17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!F18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!F19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!F20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!F21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!F22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!F23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!F24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!F25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!F26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!F27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!F28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!F29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!F30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!F31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!F32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!F33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!F3)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="11" cm="1">
+        <f t="array" ref="E2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!G3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!G4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!G5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!G6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!G7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!G8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!G9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!G10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!G11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!G12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!G13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!G14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!G15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!G16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!G17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!G18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!G19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!G20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!G21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!G22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!G23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!G24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!G25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!G26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!G27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!G28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!G29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!G30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!G31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!G32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!G33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!G3)</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="11" cm="1">
+        <f t="array" ref="F2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!H3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!H4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!H5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!H6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!H7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!H8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!H9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!H10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!H11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!H12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!H13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!H14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!H15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!H16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!H17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!H18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!H19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!H20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!H21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!H22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!H23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!H24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!H25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!H26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!H27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!H28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!H29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!H30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!H31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!H32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!H33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!H3)</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="11" cm="1">
+        <f t="array" ref="G2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!I3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!I4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!I5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!I6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!I7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!I8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!I9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!I10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!I11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!I12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!I13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!I14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!I15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!I16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!I17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!I18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!I19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!I20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!I21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!I22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!I23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!I24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!I25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!I26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!I27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!I28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!I29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!I30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!I31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!I32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!I33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!I3)</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="11" cm="1">
+        <f t="array" ref="H2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!J3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!J4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!J5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!J6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!J7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!J8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!J9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!J10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!J11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!J12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!J13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!J14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!J15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!J16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!J17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!J18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!J19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!J20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!J21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!J22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!J23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!J24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!J25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!J26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!J27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!J28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!J29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!J30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!J31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!J32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!J33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!J3)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="11" cm="1">
+        <f t="array" ref="I2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!K3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!K4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!K5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!K6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!K7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!K8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!K9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!K10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!K11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!K12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!K13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!K14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!K15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!K16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!K17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!K18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!K19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!K20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!K21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!K22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!K23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!K24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!K25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!K26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!K27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!K28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!K29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!K30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!K31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!K32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!K33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!K3)</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="11" cm="1">
+        <f t="array" ref="J2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!L3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!L4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!L5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!L6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!L7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!L8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!L9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!L10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!L11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!L12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!L13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!L14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!L15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!L16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!L17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!L18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!L19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!L20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!L21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!L22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!L23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!L24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!L25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!L26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!L27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!L28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!L29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!L30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!L31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!L32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!L33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!L3)</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="11" cm="1">
+        <f t="array" ref="K2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!M3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!M4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!M5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!M6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!M7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!M8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!M9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!M10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!M11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!M12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!M13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!M14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!M15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!M16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!M17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!M18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!M19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!M20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!M21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!M22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!M23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!M24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!M25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!M26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!M27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!M28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!M29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!M30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!M31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!M32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!M33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!M3)</f>
+        <v>1</v>
+      </c>
+      <c r="L2" s="11" cm="1">
+        <f t="array" ref="L2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!N3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!N4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!N5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!N6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!N7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!N8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!N9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!N10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!N11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!N12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!N13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!N14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!N15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!N16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!N17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!N18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!N19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!N20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!N21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!N22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!N23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!N24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!N25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!N26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!N27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!N28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!N29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!N30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!N31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!N32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!N33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!N3)</f>
+        <v>1</v>
+      </c>
+      <c r="M2" s="11" cm="1">
+        <f t="array" ref="M2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!O3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!O4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!O5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!O6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!O7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!O8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!O9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!O10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!O11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!O12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!O13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!O14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!O15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!O16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!O17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!O18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!O19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!O20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!O21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!O22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!O23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!O24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!O25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!O26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!O27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!O28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!O29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!O30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!O31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!O32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!O33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!O3)</f>
+        <v>1</v>
+      </c>
+      <c r="N2" s="11" cm="1">
+        <f t="array" ref="N2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!P3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!P4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!P5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!P6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!P7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!P8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!P9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!P10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!P11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!P12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!P13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!P14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!P15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!P16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!P17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!P18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!P19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!P20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!P21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!P22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!P23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!P24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!P25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!P26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!P27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!P28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!P29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!P30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!P31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!P32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!P33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!P3)</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="11" cm="1">
+        <f t="array" ref="O2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!Q3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!Q4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!Q5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!Q6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!Q7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!Q8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!Q9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!Q10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!Q11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!Q12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!Q13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!Q14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!Q15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!Q16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!Q17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!Q18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!Q19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!Q20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!Q21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!Q22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!Q23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!Q24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!Q25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!Q26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!Q27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!Q28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!Q29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!Q30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!Q31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!Q32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!Q33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!Q3)</f>
+        <v>1</v>
+      </c>
+      <c r="P2" s="11" cm="1">
+        <f t="array" ref="P2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!R3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!R4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!R5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!R6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!R7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!R8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!R9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!R10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!R11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!R12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!R13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!R14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!R15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!R16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!R17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!R18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!R19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!R20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!R21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!R22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!R23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!R24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!R25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!R26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!R27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!R28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!R29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!R30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!R31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!R32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!R33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!R3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="11" cm="1">
+        <f t="array" ref="Q2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!R3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!R4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!R5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!R6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!R7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!R8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!R9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!R10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!R11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!R12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!R13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!R14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!R15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!R16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!R17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!R18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!R19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!R20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!R21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!R22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!R23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!R24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!R25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!R26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!R27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!R28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!R29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!R30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!R31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!R32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!R33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!R3)</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="11" cm="1">
+        <f t="array" ref="R2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!T3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!T4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!T5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!T6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!T7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!T8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!T9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!T10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!T11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!T12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!T13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!T14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!T15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!T16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!T17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!T18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!T19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!T20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!T21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!T22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!T23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!T24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!T25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!T26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!T27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!T28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!T29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!T30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!T31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!T32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!T33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!T3)</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="11" cm="1">
+        <f t="array" ref="S2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!U3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!U4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!U5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!U6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!U7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!U8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!U9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!U10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!U11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!U12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!U13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!U14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!U15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!U16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!U17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!U18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!U19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!U20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!U21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!U22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!U23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!U24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!U25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!U26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!U27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!U28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!U29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!U30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!U31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!U32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!U33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!U3)</f>
+        <v>1</v>
+      </c>
+      <c r="T2" s="11" cm="1">
+        <f t="array" ref="T2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!V3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!V4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!V5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!V6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!V7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!V8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!V9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!V10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!V11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!V12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!V13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!V14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!V15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!V16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!V17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!V18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!V19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!V20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!V21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!V22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!V23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!V24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!V25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!V26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!V27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!V28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!V29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!V30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!V31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!V32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!V33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!V3)</f>
+        <v>1</v>
+      </c>
+      <c r="U2" s="11" cm="1">
+        <f t="array" ref="U2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!V3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!V4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!V5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!V6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!V7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!V8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!V9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!V10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!V11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!V12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!V13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!V14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!V15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!V16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!V17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!V18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!V19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!V20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!V21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!V22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!V23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!V24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!V25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!V26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!V27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!V28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!V29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!V30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!V31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!V32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!V33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!V3)</f>
+        <v>1</v>
+      </c>
+      <c r="V2" s="11" cm="1">
+        <f t="array" ref="V2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!X3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!X4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!X5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!X6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!X7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!X8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!X9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!X10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!X11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!X12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!X13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!X14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!X15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!X16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!X17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!X18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!X19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!X20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!X21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!X22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!X23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!X24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!X25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!X26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!X27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!X28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!X29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!X30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!X31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!X32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!X33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!X3)</f>
+        <v>1</v>
+      </c>
+      <c r="W2" s="11" cm="1">
+        <f t="array" ref="W2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!Y3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!Y4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!Y5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!Y6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!Y7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!Y8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!Y9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!Y10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!Y11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!Y12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!Y13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!Y14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!Y15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!Y16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!Y17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!Y18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!Y19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!Y20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!Y21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!Y22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!Y23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!Y24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!Y25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!Y26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!Y27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!Y28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!Y29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!Y30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!Y31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!Y32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!Y33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!Y3)</f>
+        <v>1</v>
+      </c>
+      <c r="X2" s="11" cm="1">
+        <f t="array" ref="X2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!Z3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!Z4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!Z5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!Z6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!Z7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!Z8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!Z9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!Z10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!Z11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!Z12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!Z13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!Z14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!Z15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!Z16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!Z17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!Z18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!Z19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!Z20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!Z21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!Z22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!Z23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!Z24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!Z25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!Z26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!Z27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!Z28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!Z29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!Z30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!Z31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!Z32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!Z33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!Z3)</f>
+        <v>1</v>
+      </c>
+      <c r="Y2" s="11" cm="1">
+        <f t="array" ref="Y2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!AA3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!AA4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!AA5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!AA6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!AA7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!AA8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!AA9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!AA10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!AA11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!AA12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!AA13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!AA14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!AA15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!AA16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!AA17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!AA18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!AA19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!AA20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!AA21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!AA22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!AA23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!AA24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!AA25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!AA26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!AA27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!AA28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!AA29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!AA30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!AA31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!AA32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!AA33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!AA3)</f>
+        <v>0</v>
+      </c>
+      <c r="Z2" s="11" cm="1">
+        <f t="array" ref="Z2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AB3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AB4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AB5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AB6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AB7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AB8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AB9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AB10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AB11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AB12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AB13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AB14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AB15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AB16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AB17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AB18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AB19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AB20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AB21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AB22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AB23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AB24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AB25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AB26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AB27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AB28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AB29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AB30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AB31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AB32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AB33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AB3)</f>
+        <v>0</v>
+      </c>
+      <c r="AA2" s="11" cm="1">
+        <f t="array" ref="AA2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AC3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AC4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AC5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AC6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AC7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AC8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AC9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AC10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AC11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AC12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AC13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AC14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AC15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AC16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AC17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AC18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AC19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AC20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AC21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AC22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AC23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AC24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AC25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AC26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AC27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AC28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AC29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AC30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AC31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AC32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AC33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AC3)</f>
+        <v>0</v>
+      </c>
+      <c r="AB2" s="11" cm="1">
+        <f t="array" ref="AB2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AD3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AD4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AD5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AD6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AD7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AD8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AD9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AD10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AD11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AD12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AD13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AD14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AD15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AD16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AD17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AD18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AD19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AD20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AD21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AD22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AD23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AD24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AD25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AD26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AD27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AD28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AD29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AD30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AD31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AD32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AD33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AD3)</f>
+        <v>1</v>
+      </c>
+      <c r="AC2" s="11" cm="1">
+        <f t="array" ref="AC2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AE3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AE4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AE5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AE6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AE7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AE8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AE9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AE10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AE11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AE12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AE13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AE14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AE15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AE16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AE17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AE18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AE19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AE20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AE21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AE22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AE23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AE24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AE25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AE26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AE27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AE28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AE29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AE30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AE31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AE32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AE33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AE3)</f>
+        <v>1</v>
+      </c>
+      <c r="AD2" s="11" cm="1">
+        <f t="array" ref="AD2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AF3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AF4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AF5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AF6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AF7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AF8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AF9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AF10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AF11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AF12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AF13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AF14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AF15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AF16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AF17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AF18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AF19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AF20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AF21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AF22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AF23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AF24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AF25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AF26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AF27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AF28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AF29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AF30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AF31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AF32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AF33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AF3)</f>
+        <v>1</v>
+      </c>
+      <c r="AE2" s="11" cm="1">
+        <f t="array" ref="AE2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AG3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AG4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AG5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AG6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AG7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AG8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AG9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AG10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AG11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AG12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AG13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AG14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AG15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AG16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AG17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AG18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AG19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AG20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AG21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AG22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AG23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AG24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AG25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AG26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AG27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AG28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AG29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AG30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AG31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AG32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AG33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AG3)</f>
+        <v>1</v>
+      </c>
+      <c r="AF2" s="11" cm="1">
+        <f t="array" ref="AF2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AH3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AH4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AH5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AH6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AH7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AH8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AH9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AH10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AH11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AH12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AH13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AH14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AH15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AH16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AH17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AH18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AH19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AH20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AH21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AH22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AH23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AH24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AH25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AH26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AH27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AH28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AH29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AH30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AH31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AH32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AH33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AH3)</f>
+        <v>1</v>
+      </c>
+      <c r="AG2" s="11" cm="1">
+        <f t="array" ref="AG2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AI3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AI4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AI5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AI6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AI7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AI8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AI9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AI10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AI11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AI12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AI13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AI14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AI15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AI16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AI17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AI18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AI19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AI20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AI21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AI22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AI23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AI24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AI25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AI26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AI27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AI28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AI29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AI30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AI31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AI32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AI33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AI3)</f>
+        <v>1</v>
+      </c>
+      <c r="AH2" s="11" cm="1">
+        <f t="array" ref="AH2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AJ3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AJ4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AJ5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AJ6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AJ7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AJ8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AJ9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AJ10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AJ11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AJ12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AJ13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AJ14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AJ15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AJ16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AJ17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AJ18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AJ19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AJ20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AJ21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AJ22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AJ23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AJ24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AJ25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AJ26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AJ27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AJ28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AJ29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AJ30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AJ31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AJ32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AJ33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AJ3)</f>
+        <v>0</v>
+      </c>
+      <c r="AI2" s="11" cm="1">
+        <f t="array" ref="AI2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AK3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AK4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AK5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AK6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AK7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AK8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AK9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AK10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AK11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AK12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AK13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AK14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AK15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AK16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AK17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AK18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AK19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AK20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AK21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AK22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AK23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AK24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AK25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AK26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AK27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AK28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AK29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AK30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AK31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AK32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AK33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AK3)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="11" cm="1">
+        <f t="array" ref="AJ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AL3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AL4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AL5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AL6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AL7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AL8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AL9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AL10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AL11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AL12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AL13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AL14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AL15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AL16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AL17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AL18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AL19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AL20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AL21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AL22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AL23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AL24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AL25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AL26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AL27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AL28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AL29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AL30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AL31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AL32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AL33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AL3)</f>
+        <v>0</v>
+      </c>
+      <c r="AK2" s="11" cm="1">
+        <f t="array" ref="AK2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AM3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AM4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AM5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AM6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AM7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AM8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AM9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AM10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AM11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AM12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AM13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AM14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AM15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AM16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AM17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AM18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AM19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AM20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AM21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AM22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AM23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AM24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AM25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AM26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AM27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AM28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AM29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AM30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AM31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AM32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AM33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AM3)</f>
+        <v>1</v>
+      </c>
+      <c r="AL2" s="11" cm="1">
+        <f t="array" ref="AL2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AN3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AN4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AN5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AN6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AN7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AN8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AN9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AN10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AN11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AN12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AN13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AN14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AN15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AN16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AN17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AN18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AN19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AN20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AN21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AN22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AN23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AN24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AN25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AN26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AN27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AN28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AN29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AN30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AN31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AN32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AN33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AN3)</f>
+        <v>1</v>
+      </c>
+      <c r="AM2" s="11" cm="1">
+        <f t="array" ref="AM2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AO3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AO4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AO5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AO6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AO7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AO8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AO9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AO10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AO11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AO12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AO13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AO14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AO15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AO16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AO17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AO18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AO19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AO20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AO21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AO22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AO23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AO24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AO25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AO26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AO27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AO28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AO29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AO30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AO31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AO32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AO33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AO3)</f>
+        <v>1</v>
+      </c>
+      <c r="AN2" s="11" cm="1">
+        <f t="array" ref="AN2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AP3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AP4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AP5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AP6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AP7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AP8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AP9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AP10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AP11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AP12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AP13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AP14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AP15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AP16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AP17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AP18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AP19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AP20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AP21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AP22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AP23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AP24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AP25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AP26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AP27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AP28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AP29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AP30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AP31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AP32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AP33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AP3)</f>
+        <v>1</v>
+      </c>
+      <c r="AO2" s="11" cm="1">
+        <f t="array" ref="AO2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AQ3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AQ4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AQ5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AQ6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AQ7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AQ8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AQ9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AQ10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AQ11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AQ12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AQ13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AQ14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AQ15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AQ16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AQ17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AQ18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AQ19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AQ20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AQ21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AQ22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AQ23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AQ24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AQ25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AQ26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AQ27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AQ28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AQ29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AQ30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AQ31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AQ32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AQ33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AQ3)</f>
+        <v>1</v>
+      </c>
+      <c r="AP2" s="11" cm="1">
+        <f t="array" ref="AP2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AR3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AR4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AR5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AR6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AR7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AR8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AR9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AR10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AR11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AR12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AR13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AR14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AR15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AR16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AR17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AR18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AR19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AR20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AR21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AR22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AR23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AR24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AR25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AR26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AR27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AR28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AR29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AR30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AR31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AR32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AR33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AR3)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="11" cm="1">
+        <f t="array" ref="AQ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AS3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AS4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AS5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AS6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AS7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AS8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AS9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AS10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AS11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AS12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AS13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AS14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AS15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AS16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AS17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AS18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AS19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AS20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AS21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AS22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AS23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AS24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AS25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AS26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AS27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AS28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AS29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AS30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AS31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AS32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AS33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AS3)</f>
+        <v>0</v>
+      </c>
+      <c r="AR2" s="11" cm="1">
+        <f t="array" ref="AR2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AS3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AS4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AS5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AS6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AS7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AS8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AS9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AS10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AS11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AS12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AS13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AS14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AS15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AS16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AS17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AS18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AS19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AS20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AS21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AS22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AS23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AS24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AS25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AS26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AS27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AS28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AS29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AS30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AS31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AS32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AS33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AS3)</f>
+        <v>0</v>
+      </c>
+      <c r="AS2" s="11" cm="1">
+        <f t="array" ref="AS2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!AU3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!AU4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!AU5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!AU6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!AU7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!AU8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!AU9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!AU10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!AU11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!AU12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!AU13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!AU14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!AU15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!AU16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!AU17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!AU18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!AU19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!AU20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!AU21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!AU22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!AU23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!AU24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!AU25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!AU26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!AU27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!AU28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!AU29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!AU30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!AU31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!AU32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!AU33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!AU3)</f>
+        <v>0</v>
+      </c>
+      <c r="AT2" s="11" cm="1">
+        <f t="array" ref="AT2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AV3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AV4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AV5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AV6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AV7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AV8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AV9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AV10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AV11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AV12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AV13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AV14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AV15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AV16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AV17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AV18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AV19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AV20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AV21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AV22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AV23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AV24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AV25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AV26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AV27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AV28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AV29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AV30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AV31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AV32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AV33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AV3)</f>
+        <v>1</v>
+      </c>
+      <c r="AU2" s="11" cm="1">
+        <f t="array" ref="AU2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AW3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AW4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AW5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AW6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AW7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AW8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AW9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AW10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AW11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AW12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AW13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AW14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AW15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AW16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AW17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AW18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AW19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AW20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AW21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AW22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AW23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AW24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AW25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AW26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AW27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AW28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AW29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AW30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AW31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AW32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AW33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AW3)</f>
+        <v>1</v>
+      </c>
+      <c r="AV2" s="11" cm="1">
+        <f t="array" ref="AV2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AX3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AX4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AX5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AX6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AX7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AX8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AX9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AX10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AX11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AX12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AX13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AX14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AX15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AX16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AX17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AX18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AX19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AX20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AX21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AX22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AX23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AX24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AX25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AX26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AX27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AX28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AX29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AX30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AX31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AX32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AX33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AX3)</f>
+        <v>1</v>
+      </c>
+      <c r="AW2" s="11" cm="1">
+        <f t="array" ref="AW2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AY3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AY4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AY5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AY6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AY7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AY8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AY9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AY10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AY11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AY12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AY13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AY14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AY15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AY16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AY17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AY18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AY19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AY20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AY21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AY22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AY23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AY24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AY25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AY26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AY27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AY28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AY29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AY30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AY31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AY32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AY33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AY3)</f>
+        <v>1</v>
+      </c>
+      <c r="AX2" s="11" cm="1">
+        <f t="array" ref="AX2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!AZ3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!AZ4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!AZ5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!AZ6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!AZ7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!AZ8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!AZ9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!AZ10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!AZ11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!AZ12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!AZ13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!AZ14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!AZ15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!AZ16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!AZ17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!AZ18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!AZ19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!AZ20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!AZ21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!AZ22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!AZ23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!AZ24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!AZ25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!AZ26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!AZ27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!AZ28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!AZ29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!AZ30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!AZ31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!AZ32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!AZ33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!AZ3)</f>
+        <v>1</v>
+      </c>
+      <c r="AY2" s="11" cm="1">
+        <f t="array" ref="AY2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BA3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BA4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BA5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BA6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BA7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BA8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BA9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BA10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BA11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BA12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BA13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BA14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BA15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BA16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BA17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BA18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BA19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BA20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BA21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BA22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BA23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BA24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BA25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BA26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BA27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BA28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BA29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BA30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BA31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BA32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BA33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BA3)</f>
+        <v>1</v>
+      </c>
+      <c r="AZ2" s="11" cm="1">
+        <f t="array" ref="AZ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BB3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BB4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BB5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BB6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BB7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BB8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BB9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BB10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BB11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BB12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BB13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BB14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BB15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BB16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BB17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BB18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BB19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BB20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BB21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BB22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BB23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BB24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BB25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BB26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BB27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BB28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BB29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BB30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BB31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BB32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BB33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BB3)</f>
+        <v>0</v>
+      </c>
+      <c r="BA2" s="11" cm="1">
+        <f t="array" ref="BA2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BC3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BC4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BC5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BC6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BC7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BC8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BC9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BC10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BC11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BC12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BC13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BC14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BC15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BC16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BC17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BC18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BC19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BC20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BC21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BC22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BC23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BC24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BC25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BC26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BC27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BC28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BC29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BC30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BC31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BC32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BC33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BC3)</f>
+        <v>0</v>
+      </c>
+      <c r="BB2" s="11" cm="1">
+        <f t="array" ref="BB2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BD3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BD4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BD5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BD6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BD7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BD8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BD9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BD10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BD11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BD12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BD13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BD14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BD15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BD16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BD17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BD18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BD19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BD20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BD21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BD22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BD23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BD24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BD25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BD26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BD27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BD28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BD29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BD30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BD31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BD32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BD33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BD3)</f>
+        <v>0</v>
+      </c>
+      <c r="BC2" s="11" cm="1">
+        <f t="array" ref="BC2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BE3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BE4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BE5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BE6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BE7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BE8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BE9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BE10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BE11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BE12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BE13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BE14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BE15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BE16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BE17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BE18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BE19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BE20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BE21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BE22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BE23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BE24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BE25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BE26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BE27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BE28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BE29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BE30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BE31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BE32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BE33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BE3)</f>
+        <v>1</v>
+      </c>
+      <c r="BD2" s="11" cm="1">
+        <f t="array" ref="BD2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BF3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BF4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BF5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BF6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BF7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BF8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BF9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BF10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BF11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BF12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BF13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BF14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BF15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BF16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BF17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BF18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BF19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BF20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BF21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BF22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BF23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BF24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BF25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BF26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BF27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BF28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BF29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BF30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BF31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BF32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BF33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BF3)</f>
+        <v>1</v>
+      </c>
+      <c r="BE2" s="11" cm="1">
+        <f t="array" ref="BE2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BG3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BG4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BG5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BG6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BG7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BG8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BG9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BG10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BG11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BG12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BG13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BG14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BG15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BG16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BG17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BG18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BG19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BG20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BG21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BG22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BG23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BG24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BG25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BG26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BG27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BG28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BG29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BG30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BG31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BG32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BG33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BG3)</f>
+        <v>1</v>
+      </c>
+      <c r="BF2" s="11" cm="1">
+        <f t="array" ref="BF2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BH3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BH4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BH5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BH6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BH7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BH8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BH9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BH10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BH11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BH12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BH13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BH14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BH15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BH16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BH17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BH18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BH19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BH20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BH21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BH22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BH23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BH24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BH25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BH26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BH27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BH28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BH29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BH30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BH31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BH32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BH33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BH3)</f>
+        <v>1</v>
+      </c>
+      <c r="BG2" s="11" cm="1">
+        <f t="array" ref="BG2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BI3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BI4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BI5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BI6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BI7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BI8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BI9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BI10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BI11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BI12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BI13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BI14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BI15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BI16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BI17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BI18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BI19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BI20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BI21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BI22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BI23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BI24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BI25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BI26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BI27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BI28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BI29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BI30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BI31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BI32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BI33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BI3)</f>
+        <v>1</v>
+      </c>
+      <c r="BH2" s="11" cm="1">
+        <f t="array" ref="BH2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BJ3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BJ4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BJ5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BJ6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BJ7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BJ8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BJ9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BJ10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BJ11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BJ12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BJ13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BJ14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BJ15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BJ16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BJ17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BJ18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BJ19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BJ20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BJ21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BJ22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BJ23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BJ24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BJ25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BJ26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BJ27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BJ28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BJ29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BJ30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BJ31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BJ32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BJ33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BJ3)</f>
+        <v>1</v>
+      </c>
+      <c r="BI2" s="11" cm="1">
+        <f t="array" ref="BI2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BK3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BK4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BK5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BK6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BK7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BK8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BK9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BK10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BK11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BK12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BK13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BK14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BK15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BK16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BK17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BK18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BK19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BK20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BK21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BK22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BK23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BK24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BK25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BK26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BK27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BK28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BK29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BK30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BK31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BK32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BK33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BK3)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ2" s="11" cm="1">
+        <f t="array" ref="BJ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BL3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BL4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BL5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BL6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BL7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BL8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BL9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BL10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BL11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BL12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BL13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BL14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BL15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BL16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BL17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BL18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BL19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BL20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BL21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BL22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BL23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BL24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BL25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BL26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BL27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BL28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BL29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BL30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BL31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BL32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BL33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BL3)</f>
+        <v>0</v>
+      </c>
+      <c r="BK2" s="11" cm="1">
+        <f t="array" ref="BK2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BM3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BM4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BM5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BM6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BM7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BM8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BM9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BM10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BM11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BM12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BM13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BM14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BM15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BM16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BM17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BM18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BM19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BM20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BM21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BM22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BM23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BM24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BM25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BM26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BM27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BM28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BM29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BM30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BM31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BM32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BM33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BM3)</f>
+        <v>0</v>
+      </c>
+      <c r="BL2" s="11" cm="1">
+        <f t="array" ref="BL2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BN3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BN4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BN5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BN6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BN7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BN8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BN9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BN10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BN11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BN12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BN13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BN14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BN15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BN16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BN17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BN18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BN19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BN20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BN21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BN22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BN23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BN24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BN25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BN26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BN27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BN28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BN29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BN30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BN31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BN32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BN33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BN3)</f>
+        <v>1</v>
+      </c>
+      <c r="BM2" s="11" cm="1">
+        <f t="array" ref="BM2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BO3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BO4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BO5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BO6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BO7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BO8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BO9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BO10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BO11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BO12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BO13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BO14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BO15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BO16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BO17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BO18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BO19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BO20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BO21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BO22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BO23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BO24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BO25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BO26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BO27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BO28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BO29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BO30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BO31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BO32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BO33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BO3)</f>
+        <v>1</v>
+      </c>
+      <c r="BN2" s="11" cm="1">
+        <f t="array" ref="BN2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BP3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BP4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BP5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BP6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BP7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BP8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BP9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BP10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BP11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BP12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BP13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BP14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BP15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BP16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BP17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BP18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BP19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BP20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BP21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BP22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BP23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BP24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BP25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BP26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BP27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BP28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BP29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BP30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BP31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BP32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BP33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BP3)</f>
+        <v>1</v>
+      </c>
+      <c r="BO2" s="11" cm="1">
+        <f t="array" ref="BO2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BQ3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BQ4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BQ5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BQ6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BQ7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BQ8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BQ9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BQ10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BQ11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BQ12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BQ13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BQ14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BQ15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BQ16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BQ17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BQ18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BQ19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BQ20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BQ21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BQ22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BQ23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BQ24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BQ25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BQ26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BQ27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BQ28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BQ29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BQ30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BQ31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BQ32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BQ33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BQ3)</f>
+        <v>1</v>
+      </c>
+      <c r="BP2" s="11" cm="1">
+        <f t="array" ref="BP2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BR3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BR4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BR5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BR6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BR7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BR8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BR9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BR10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BR11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BR12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BR13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BR14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BR15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BR16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BR17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BR18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BR19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BR20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BR21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BR22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BR23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BR24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BR25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BR26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BR27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BR28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BR29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BR30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BR31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BR32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BR33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BR3)</f>
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="11" cm="1">
+        <f t="array" ref="BQ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BS3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BS4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BS5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BS6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BS7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BS8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BS9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BS10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BS11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BS12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BS13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BS14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BS15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BS16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BS17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BS18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BS19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BS20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BS21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BS22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BS23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BS24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BS25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BS26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BS27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BS28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BS29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BS30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BS31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BS32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BS33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BS3)</f>
+        <v>1</v>
+      </c>
+      <c r="BR2" s="11" cm="1">
+        <f t="array" ref="BR2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BT3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BT4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BT5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BT6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BT7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BT8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BT9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BT10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BT11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BT12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BT13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BT14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BT15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BT16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BT17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BT18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BT19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BT20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BT21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BT22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BT23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BT24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BT25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BT26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BT27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BT28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BT29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BT30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BT31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BT32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BT33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BT3)</f>
+        <v>0</v>
+      </c>
+      <c r="BS2" s="11" cm="1">
+        <f t="array" ref="BS2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BU3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BU4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BU5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BU6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BU7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BU8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BU9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BU10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BU11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BU12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BU13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BU14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BU15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BU16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BU17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BU18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BU19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BU20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BU21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BU22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BU23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BU24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BU25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BU26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BU27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BU28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BU29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BU30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BU31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BU32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BU33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BU3)</f>
+        <v>0</v>
+      </c>
+      <c r="BT2" s="11" cm="1">
+        <f t="array" ref="BT2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BV3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BV4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BV5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BV6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BV7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BV8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BV9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BV10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BV11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BV12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BV13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BV14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BV15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BV16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BV17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BV18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BV19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BV20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BV21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BV22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BV23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BV24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BV25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BV26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BV27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BV28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BV29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BV30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BV31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BV32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BV33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BV3)</f>
+        <v>0</v>
+      </c>
+      <c r="BU2" s="11" cm="1">
+        <f t="array" ref="BU2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BW3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BW4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BW5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BW6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BW7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BW8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BW9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BW10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BW11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BW12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BW13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BW14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BW15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BW16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BW17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BW18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BW19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BW20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BW21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BW22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BW23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BW24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BW25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BW26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BW27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BW28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BW29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BW30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BW31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BW32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BW33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BW3)</f>
+        <v>1</v>
+      </c>
+      <c r="BV2" s="11" cm="1">
+        <f t="array" ref="BV2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BX3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BX4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BX5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BX6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BX7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BX8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BX9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BX10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BX11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BX12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BX13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BX14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BX15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BX16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BX17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BX18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BX19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BX20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BX21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BX22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BX23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BX24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BX25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BX26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BX27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BX28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BX29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BX30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BX31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BX32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BX33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BX3)</f>
+        <v>1</v>
+      </c>
+      <c r="BW2" s="11" cm="1">
+        <f t="array" ref="BW2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BY3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BY4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BY5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BY6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BY7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BY8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BY9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BY10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BY11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BY12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BY13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BY14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BY15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BY16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BY17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BY18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BY19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BY20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BY21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BY22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BY23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BY24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BY25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BY26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BY27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BY28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BY29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BY30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BY31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BY32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BY33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BY3)</f>
+        <v>1</v>
+      </c>
+      <c r="BX2" s="11" cm="1">
+        <f t="array" ref="BX2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BZ3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BZ4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BZ5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BZ6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BZ7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BZ8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BZ9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BZ10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BZ11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BZ12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BZ13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BZ14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BZ15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BZ16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BZ17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BZ18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BZ19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BZ20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BZ21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BZ22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BZ23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BZ24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BZ25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BZ26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BZ27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BZ28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BZ29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BZ30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BZ31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BZ32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BZ33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BZ3)</f>
+        <v>1</v>
+      </c>
+      <c r="BY2" s="11" cm="1">
+        <f t="array" ref="BY2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CA3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CA4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CA5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CA6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CA7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CA8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CA9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CA10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CA11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CA12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CA13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CA14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CA15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CA16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CA17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CA18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CA19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CA20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CA21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CA22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CA23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CA24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CA25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CA26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CA27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CA28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CA29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CA30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CA31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CA32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CA33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CA3)</f>
+        <v>1</v>
+      </c>
+      <c r="BZ2" s="11" cm="1">
+        <f t="array" ref="BZ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CB3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CB4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CB5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CB6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CB7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CB8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CB9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CB10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CB11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CB12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CB13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CB14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CB15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CB16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CB17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CB18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CB19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CB20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CB21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CB22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CB23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CB24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CB25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CB26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CB27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CB28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CB29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CB30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CB31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CB32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CB33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CB3)</f>
+        <v>1</v>
+      </c>
+      <c r="CA2" s="11" cm="1">
+        <f t="array" ref="CA2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CC3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CC4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CC5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CC6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CC7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CC8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CC9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CC10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CC11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CC12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CC13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CC14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CC15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CC16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CC17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CC18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CC19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CC20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CC21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CC22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CC23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CC24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CC25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CC26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CC27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CC28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CC29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CC30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CC31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CC32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CC33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CC3)</f>
+        <v>0</v>
+      </c>
+      <c r="CB2" s="11" cm="1">
+        <f t="array" ref="CB2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CD3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CD4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CD5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CD6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CD7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CD8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CD9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CD10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CD11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CD12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CD13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CD14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CD15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CD16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CD17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CD18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CD19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CD20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CD21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CD22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CD23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CD24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CD25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CD26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CD27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CD28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CD29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CD30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CD31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CD32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CD33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CD3)</f>
+        <v>0</v>
+      </c>
+      <c r="CC2" s="11" cm="1">
+        <f t="array" ref="CC2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CE3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CE4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CE5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CE6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CE7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CE8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CE9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CE10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CE11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CE12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CE13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CE14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CE15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CE16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CE17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CE18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CE19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CE20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CE21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CE22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CE23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CE24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CE25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CE26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CE27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CE28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CE29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CE30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CE31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CE32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CE33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CE3)</f>
+        <v>0</v>
+      </c>
+      <c r="CD2" s="11" cm="1">
+        <f t="array" ref="CD2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CF3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CF4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CF5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CF6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CF7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CF8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CF9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CF10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CF11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CF12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CF13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CF14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CF15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CF16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CF17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CF18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CF19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CF20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CF21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CF22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CF23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CF24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CF25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CF26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CF27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CF28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CF29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CF30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CF31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CF32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CF33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CF3)</f>
+        <v>1</v>
+      </c>
+      <c r="CE2" s="11" cm="1">
+        <f t="array" ref="CE2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CG3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CG4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CG5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CG6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CG7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CG8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CG9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CG10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CG11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CG12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CG13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CG14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CG15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CG16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CG17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CG18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CG19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CG20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CG21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CG22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CG23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CG24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CG25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CG26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CG27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CG28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CG29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CG30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CG31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CG32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CG33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CG3)</f>
+        <v>1</v>
+      </c>
+      <c r="CF2" s="11" cm="1">
+        <f t="array" ref="CF2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CH3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CH4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CH5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CH6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CH7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CH8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CH9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CH10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CH11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CH12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CH13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CH14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CH15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CH16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CH17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CH18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CH19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CH20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CH21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CH22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CH23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CH24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CH25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CH26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CH27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CH28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CH29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CH30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CH31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CH32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CH33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CH3)</f>
+        <v>1</v>
+      </c>
+      <c r="CG2" s="11" cm="1">
+        <f t="array" ref="CG2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CI3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CI4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CI5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CI6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CI7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CI8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CI9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CI10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CI11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CI12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CI13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CI14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CI15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CI16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CI17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CI18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CI19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CI20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CI21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CI22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CI23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CI24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CI25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CI26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CI27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CI28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CI29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CI30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CI31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CI32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CI33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CI3)</f>
+        <v>1</v>
+      </c>
+      <c r="CH2" s="11" cm="1">
+        <f t="array" ref="CH2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CJ3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CJ4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CJ5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CJ6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CJ7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CJ8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CJ9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CJ10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CJ11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CJ12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CJ13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CJ14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CJ15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CJ16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CJ17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CJ18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CJ19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CJ20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CJ21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CJ22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CJ23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CJ24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CJ25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CJ26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CJ27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CJ28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CJ29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CJ30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CJ31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CJ32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CJ33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CJ3)</f>
+        <v>1</v>
+      </c>
+      <c r="CI2" s="11" cm="1">
+        <f t="array" ref="CI2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CK3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CK4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CK5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CK6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CK7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CK8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CK9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CK10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CK11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CK12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CK13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CK14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CK15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CK16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CK17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CK18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CK19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CK20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CK21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CK22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CK23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CK24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CK25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CK26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CK27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CK28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CK29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CK30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CK31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CK32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CK33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CK3)</f>
+        <v>1</v>
+      </c>
+      <c r="CJ2" s="11" cm="1">
+        <f t="array" ref="CJ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CL3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CL4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CL5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CL6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CL7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CL8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CL9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CL10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CL11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CL12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CL13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CL14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CL15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CL16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CL17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CL18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CL19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CL20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CL21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CL22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CL23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CL24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CL25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CL26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CL27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CL28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CL29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CL30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CL31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CL32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CL33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CL3)</f>
+        <v>0</v>
+      </c>
+      <c r="CK2" s="11" cm="1">
+        <f t="array" ref="CK2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CM3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CM4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CM5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CM6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CM7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CM8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CM9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CM10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CM11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CM12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CM13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CM14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CM15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CM16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CM17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CM18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CM19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CM20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CM21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CM22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CM23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CM24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CM25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CM26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CM27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CM28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CM29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CM30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CM31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CM32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CM33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CM3)</f>
+        <v>0</v>
+      </c>
+      <c r="CL2" s="11" cm="1">
+        <f t="array" ref="CL2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CN3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CN4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CN5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CN6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CN7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CN8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CN9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CN10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CN11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CN12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CN13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CN14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CN15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CN16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CN17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CN18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CN19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CN20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CN21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CN22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CN23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CN24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CN25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CN26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CN27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CN28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CN29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CN30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CN31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CN32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CN33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CN3)</f>
+        <v>0</v>
+      </c>
+      <c r="CM2" s="11" cm="1">
+        <f t="array" ref="CM2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CO3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CO4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CO5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CO6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CO7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CO8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CO9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CO10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CO11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CO12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CO13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CO14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CO15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CO16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CO17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CO18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CO19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CO20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CO21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CO22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CO23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CO24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CO25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CO26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CO27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CO28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CO29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CO30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CO31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CO32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CO33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CO3)</f>
+        <v>1</v>
+      </c>
+      <c r="CN2" s="11" cm="1">
+        <f t="array" ref="CN2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CP3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CP4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CP5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CP6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CP7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CP8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CP9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CP10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CP11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CP12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CP13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CP14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CP15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CP16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CP17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CP18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CP19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CP20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CP21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CP22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CP23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CP24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CP25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CP26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CP27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CP28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CP29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CP30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CP31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CP32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CP33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CP3)</f>
+        <v>1</v>
+      </c>
+      <c r="CO2" s="11" cm="1">
+        <f t="array" ref="CO2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CQ3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CQ4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CQ5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CQ6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CQ7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CQ8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CQ9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CQ10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CQ11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CQ12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CQ13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CQ14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CQ15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CQ16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CQ17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CQ18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CQ19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CQ20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CQ21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CQ22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CQ23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CQ24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CQ25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CQ26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CQ27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CQ28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CQ29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CQ30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CQ31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CQ32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CQ33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CQ3)</f>
+        <v>1</v>
+      </c>
+      <c r="CP2" s="11" cm="1">
+        <f t="array" ref="CP2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CR3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CR4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CR5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CR6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CR7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CR8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CR9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CR10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CR11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CR12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CR13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CR14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CR15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CR16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CR17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CR18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CR19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CR20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CR21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CR22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CR23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CR24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CR25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CR26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CR27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CR28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CR29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CR30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CR31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CR32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CR33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CR3)</f>
+        <v>1</v>
+      </c>
+      <c r="CQ2" s="11" cm="1">
+        <f t="array" ref="CQ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CS3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CS4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CS5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CS6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CS7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CS8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CS9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CS10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CS11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CS12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CS13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CS14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CS15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CS16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CS17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CS18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CS19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CS20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CS21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CS22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CS23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CS24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CS25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CS26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CS27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CS28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CS29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CS30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CS31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CS32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CS33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CS3)</f>
+        <v>1</v>
+      </c>
+      <c r="CR2" s="11" cm="1">
+        <f t="array" ref="CR2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CT3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CT4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CT5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CT6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CT7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CT8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CT9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CT10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CT11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CT12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CT13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CT14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CT15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CT16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CT17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CT18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CT19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CT20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CT21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CT22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CT23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CT24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CT25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CT26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CT27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CT28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CT29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CT30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CT31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CT32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CT33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CT3)</f>
+        <v>1</v>
+      </c>
+      <c r="CS2" s="11" cm="1">
+        <f t="array" ref="CS2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CU3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CU4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CU5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CU6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CU7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CU8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CU9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CU10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CU11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CU12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CU13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CU14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CU15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CU16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CU17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CU18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CU19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CU20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CU21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CU22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CU23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CU24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CU25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CU26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CU27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CU28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CU29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CU30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CU31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CU32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CU33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CU3)</f>
+        <v>0</v>
+      </c>
+      <c r="CT2" s="11" cm="1">
+        <f t="array" ref="CT2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CV3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CV4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CV5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CV6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CV7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CV8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CV9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CV10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CV11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CV12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CV13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CV14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CV15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CV16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CV17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CV18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CV19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CV20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CV21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CV22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CV23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CV24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CV25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CV26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CV27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CV28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CV29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CV30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CV31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CV32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CV33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CV3)</f>
+        <v>0</v>
+      </c>
+      <c r="CU2" s="11" cm="1">
+        <f t="array" ref="CU2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CW3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CW4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CW5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CW6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CW7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CW8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CW9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CW10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CW11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CW12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CW13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CW14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CW15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CW16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CW17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CW18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CW19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CW20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CW21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CW22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CW23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CW24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CW25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CW26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CW27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CW28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CW29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CW30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CW31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CW32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CW33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CW3)</f>
+        <v>0</v>
+      </c>
+      <c r="CV2" s="11" cm="1">
+        <f t="array" ref="CV2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CX3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CX4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CX5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CX6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CX7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CX8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CX9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CX10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CX11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CX12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CX13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CX14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CX15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CX16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CX17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CX18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CX19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CX20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CX21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CX22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CX23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CX24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CX25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CX26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CX27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CX28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CX29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CX30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CX31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CX32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CX33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CX3)</f>
+        <v>1</v>
+      </c>
+      <c r="CW2" s="11" cm="1">
+        <f t="array" ref="CW2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CY3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CY4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CY5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CY6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CY7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CY8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CY9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CY10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CY11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CY12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CY13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CY14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CY15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CY16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CY17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CY18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CY19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CY20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CY21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CY22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CY23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CY24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CY25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CY26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CY27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CY28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CY29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CY30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CY31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CY32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CY33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CY3)</f>
+        <v>1</v>
+      </c>
+      <c r="CX2" s="11" cm="1">
+        <f t="array" ref="CX2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CZ3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CZ4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CZ5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CZ6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CZ7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CZ8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CZ9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CZ10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CZ11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CZ12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CZ13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CZ14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CZ15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CZ16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CZ17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CZ18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CZ19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CZ20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CZ21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CZ22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CZ23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CZ24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CZ25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CZ26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CZ27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CZ28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CZ29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CZ30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CZ31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CZ32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CZ33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CZ3)</f>
+        <v>1</v>
+      </c>
+      <c r="CY2" s="11" cm="1">
+        <f t="array" ref="CY2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!DA3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!DA4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!DA5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!DA6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!DA7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!DA8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!DA9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!DA10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!DA11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!DA12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!DA13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!DA14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!DA15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!DA16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!DA17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!DA18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!DA19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!DA20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!DA21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!DA22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!DA23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!DA24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!DA25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!DA26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!DA27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!DA28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!DA29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!DA30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!DA31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!DA32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!DA33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!DA3)</f>
+        <v>1</v>
+      </c>
+      <c r="CZ2" s="11" cm="1">
+        <f t="array" ref="CZ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!DB3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!DB4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!DB5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!DB6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!DB7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!DB8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!DB9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!DB10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!DB11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!DB12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!DB13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!DB14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!DB15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!DB16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!DB17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!DB18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!DB19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!DB20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!DB21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!DB22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!DB23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!DB24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!DB25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!DB26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!DB27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!DB28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!DB29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!DB30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!DB31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!DB32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!DB33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!DB3)</f>
+        <v>1</v>
+      </c>
+      <c r="DA2" s="11" cm="1">
+        <f t="array" ref="DA2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!DC3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!DC4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!DC5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!DC6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!DC7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!DC8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!DC9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!DC10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!DC11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!DC12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!DC13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!DC14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!DC15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!DC16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!DC17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!DC18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!DC19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!DC20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!DC21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!DC22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!DC23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!DC24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!DC25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!DC26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!DC27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!DC28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!DC29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!DC30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!DC31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!DC32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!DC33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!DC3)</f>
+        <v>1</v>
+      </c>
+      <c r="DB2" s="11" cm="1">
+        <f t="array" ref="DB2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!DD3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!DD4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!DD5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!DD6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!DD7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!DD8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!DD9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!DD10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!DD11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!DD12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!DD13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!DD14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!DD15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!DD16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!DD17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!DD18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!DD19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!DD20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!DD21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!DD22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!DD23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!DD24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!DD25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!DD26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!DD27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!DD28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!DD29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!DD30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!DD31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!DD32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!DD33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!DD3)</f>
+        <v>0</v>
+      </c>
+      <c r="DC2" s="11" cm="1">
+        <f t="array" ref="DC2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!DE3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!DE4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!DE5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!DE6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!DE7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!DE8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!DE9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!DE10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!DE11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!DE12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!DE13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!DE14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!DE15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!DE16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!DE17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!DE18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!DE19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!DE20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!DE21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!DE22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!DE23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!DE24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!DE25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!DE26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!DE27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!DE28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!DE29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!DE30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!DE31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!DE32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!DE33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!DE3)</f>
+        <v>0</v>
+      </c>
+      <c r="DD2" s="11" cm="1">
+        <f t="array" ref="DD2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!DF3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!DF4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!DF5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!DF6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!DF7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!DF8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!DF9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!DF10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!DF11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!DF12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!DF13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!DF14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!DF15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!DF16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!DF17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!DF18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!DF19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!DF20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!DF21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!DF22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!DF23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!DF24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!DF25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!DF26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!DF27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!DF28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!DF29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!DF30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!DF31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!DF32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!DF33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!DF3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="BN3" s="14"/>
+      <c r="BO3" s="14"/>
+      <c r="BP3" s="14"/>
+      <c r="BQ3" s="14"/>
+      <c r="BR3" s="14"/>
+      <c r="BS3" s="14"/>
+      <c r="BT3" s="14"/>
+      <c r="BU3" s="14"/>
+      <c r="BV3" s="14"/>
+      <c r="BW3" s="14"/>
+      <c r="BX3" s="14"/>
+      <c r="BY3" s="14"/>
+      <c r="BZ3" s="14"/>
+      <c r="CA3" s="14"/>
+      <c r="CB3" s="14"/>
+      <c r="CC3" s="14"/>
+      <c r="CD3" s="14"/>
+      <c r="CE3" s="14"/>
+      <c r="CF3" s="14"/>
+      <c r="CG3" s="14"/>
+      <c r="CH3" s="14"/>
+      <c r="CI3" s="14"/>
+      <c r="CJ3" s="14"/>
+      <c r="CK3" s="14"/>
+      <c r="CL3" s="14"/>
+      <c r="CM3" s="14"/>
+      <c r="CN3" s="14"/>
+      <c r="CO3" s="14"/>
+      <c r="CP3" s="14"/>
+      <c r="CQ3" s="14"/>
+      <c r="CR3" s="14"/>
+      <c r="CS3" s="14"/>
+      <c r="CT3" s="14"/>
+      <c r="CU3" s="14"/>
+      <c r="CV3" s="14"/>
+      <c r="CW3" s="14"/>
+      <c r="CX3" s="14"/>
+      <c r="CY3" s="14"/>
+      <c r="CZ3" s="14"/>
+      <c r="DA3" s="14"/>
+      <c r="DB3" s="14"/>
+      <c r="DC3" s="14"/>
+      <c r="DD3" s="14"/>
+    </row>
+    <row r="4" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="CO4" s="14"/>
+      <c r="CP4" s="14"/>
+      <c r="CQ4" s="14"/>
+      <c r="CR4" s="14"/>
+      <c r="CS4" s="14"/>
+      <c r="CT4" s="14"/>
+      <c r="CU4" s="14"/>
+      <c r="CV4" s="14"/>
+      <c r="CW4" s="14"/>
+      <c r="CX4" s="14"/>
+      <c r="CY4" s="14"/>
+      <c r="CZ4" s="14"/>
+      <c r="DA4" s="14"/>
+      <c r="DB4" s="14"/>
+      <c r="DC4" s="14"/>
+      <c r="DD4" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF60A41E-DB03-5F46-886C-E18FFE6E9199}">
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -22586,7 +23428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA123D2-0336-694E-A8F7-870F75EFF230}">
   <dimension ref="A1:A12"/>
   <sheetViews>

</xml_diff>

<commit_message>
datas of farmandehi added
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammad/Library/CloudStorage/OneDrive-email.kntu.ac.ir/MangerDashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76FA512-2616-E341-B19B-F7BD79FF46B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619A2899-1B16-2247-AD83-D7A610FE05AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{490754A7-E054-EF47-883C-C68C37A7F559}"/>
   </bookViews>
@@ -22538,8 +22538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10993374-1CDE-D345-894E-3CB87C699537}">
   <dimension ref="A1:DD4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="BC2" sqref="BC2"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="CR1" workbookViewId="0">
+      <selection activeCell="DD3" sqref="DD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23091,219 +23091,219 @@
         <v>0</v>
       </c>
       <c r="BC2" s="11" cm="1">
-        <f t="array" ref="BC2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BE3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BE4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BE5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BE6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BE7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BE8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BE9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BE10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BE11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BE12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BE13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BE14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BE15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BE16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BE17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BE18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BE19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BE20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BE21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BE22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BE23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BE24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BE25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BE26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BE27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BE28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BE29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BE30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BE31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BE32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BE33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BE3)</f>
+        <f t="array" ref="BC2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BE3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BE4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BE5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BE6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BE7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BE8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BE9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BE10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BE11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BE12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BE13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BE14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BE15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BE16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BE17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BE18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BE19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BE20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BE21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BE22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BE23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BE24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BE25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BE26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BE27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BE28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BE29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BE30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BE31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BE32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BE33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BE3)</f>
         <v>1</v>
       </c>
       <c r="BD2" s="11" cm="1">
-        <f t="array" ref="BD2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BF3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BF4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BF5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BF6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BF7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BF8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BF9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BF10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BF11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BF12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BF13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BF14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BF15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BF16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BF17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BF18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BF19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BF20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BF21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BF22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BF23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BF24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BF25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BF26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BF27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BF28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BF29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BF30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BF31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BF32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BF33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BF3)</f>
+        <f t="array" ref="BD2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BF3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BF4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BF5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BF6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BF7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BF8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BF9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BF10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BF11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BF12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BF13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BF14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BF15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BF16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BF17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BF18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BF19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BF20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BF21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BF22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BF23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BF24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BF25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BF26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BF27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BF28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BF29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BF30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BF31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BF32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BF33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BF3)</f>
         <v>1</v>
       </c>
       <c r="BE2" s="11" cm="1">
-        <f t="array" ref="BE2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BG3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BG4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BG5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BG6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BG7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BG8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BG9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BG10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BG11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BG12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BG13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BG14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BG15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BG16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BG17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BG18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BG19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BG20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BG21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BG22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BG23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BG24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BG25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BG26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BG27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BG28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BG29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BG30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BG31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BG32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BG33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BG3)</f>
+        <f t="array" ref="BE2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BG3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BG4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BG5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BG6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BG7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BG8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BG9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BG10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BG11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BG12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BG13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BG14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BG15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BG16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BG17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BG18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BG19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BG20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BG21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BG22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BG23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BG24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BG25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BG26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BG27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BG28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BG29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BG30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BG31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BG32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BG33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BG3)</f>
         <v>1</v>
       </c>
       <c r="BF2" s="11" cm="1">
-        <f t="array" ref="BF2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BH3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BH4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BH5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BH6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BH7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BH8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BH9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BH10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BH11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BH12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BH13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BH14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BH15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BH16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BH17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BH18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BH19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BH20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BH21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BH22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BH23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BH24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BH25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BH26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BH27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BH28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BH29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BH30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BH31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BH32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BH33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BH3)</f>
+        <f t="array" ref="BF2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BH3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BH4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BH5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BH6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BH7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BH8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BH9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BH10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BH11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BH12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BH13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BH14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BH15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BH16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BH17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BH18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BH19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BH20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BH21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BH22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BH23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BH24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BH25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BH26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BH27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BH28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BH29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BH30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BH31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BH32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BH33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BH3)</f>
         <v>1</v>
       </c>
       <c r="BG2" s="11" cm="1">
-        <f t="array" ref="BG2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BI3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BI4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BI5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BI6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BI7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BI8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BI9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BI10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BI11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BI12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BI13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BI14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BI15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BI16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BI17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BI18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BI19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BI20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BI21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BI22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BI23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BI24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BI25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BI26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BI27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BI28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BI29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BI30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BI31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BI32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BI33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BI3)</f>
+        <f t="array" ref="BG2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BI3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BI4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BI5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BI6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BI7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BI8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BI9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BI10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BI11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BI12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BI13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BI14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BI15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BI16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BI17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BI18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BI19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BI20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BI21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BI22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BI23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BI24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BI25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BI26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BI27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BI28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BI29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BI30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BI31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BI32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BI33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BI3)</f>
         <v>1</v>
       </c>
       <c r="BH2" s="11" cm="1">
-        <f t="array" ref="BH2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BJ3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BJ4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BJ5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BJ6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BJ7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BJ8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BJ9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BJ10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BJ11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BJ12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BJ13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BJ14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BJ15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BJ16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BJ17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BJ18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BJ19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BJ20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BJ21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BJ22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BJ23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BJ24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BJ25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BJ26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BJ27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BJ28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BJ29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BJ30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BJ31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BJ32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BJ33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BJ3)</f>
+        <f t="array" ref="BH2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BJ3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BJ4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BJ5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BJ6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BJ7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BJ8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BJ9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BJ10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BJ11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BJ12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BJ13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BJ14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BJ15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BJ16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BJ17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BJ18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BJ19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BJ20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BJ21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BJ22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BJ23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BJ24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BJ25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BJ26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BJ27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BJ28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BJ29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BJ30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BJ31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BJ32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BJ33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BJ3)</f>
         <v>1</v>
       </c>
       <c r="BI2" s="11" cm="1">
-        <f t="array" ref="BI2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BK3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BK4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BK5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BK6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BK7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BK8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BK9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BK10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BK11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BK12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BK13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BK14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BK15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BK16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BK17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BK18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BK19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BK20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BK21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BK22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BK23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BK24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BK25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BK26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BK27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BK28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BK29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BK30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BK31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BK32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BK33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BK3)</f>
+        <f t="array" ref="BI2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BK3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BK4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BK5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BK6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BK7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BK8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BK9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BK10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BK11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BK12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BK13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BK14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BK15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BK16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BK17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BK18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BK19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BK20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BK21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BK22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BK23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BK24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BK25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BK26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BK27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BK28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BK29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BK30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BK31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BK32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BK33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BK3)</f>
         <v>0</v>
       </c>
       <c r="BJ2" s="11" cm="1">
-        <f t="array" ref="BJ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BL3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BL4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BL5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BL6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BL7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BL8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BL9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BL10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BL11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BL12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BL13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BL14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BL15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BL16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BL17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BL18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BL19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BL20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BL21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BL22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BL23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BL24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BL25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BL26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BL27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BL28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BL29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BL30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BL31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BL32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BL33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BL3)</f>
+        <f t="array" ref="BJ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BL3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BL4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BL5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BL6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BL7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BL8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BL9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BL10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BL11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BL12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BL13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BL14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BL15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BL16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BL17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BL18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BL19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BL20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BL21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BL22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BL23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BL24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BL25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BL26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BL27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BL28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BL29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BL30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BL31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BL32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BL33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BL3)</f>
         <v>0</v>
       </c>
       <c r="BK2" s="11" cm="1">
-        <f t="array" ref="BK2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BM3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BM4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BM5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BM6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BM7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BM8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BM9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BM10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BM11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BM12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BM13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BM14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BM15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BM16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BM17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BM18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BM19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BM20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BM21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BM22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BM23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BM24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BM25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BM26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BM27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BM28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BM29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BM30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BM31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BM32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BM33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BM3)</f>
+        <f t="array" ref="BK2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BM3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BM4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BM5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BM6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BM7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BM8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BM9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BM10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BM11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BM12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BM13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BM14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BM15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BM16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BM17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BM18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BM19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BM20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BM21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BM22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BM23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BM24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BM25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BM26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BM27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BM28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BM29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BM30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BM31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BM32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BM33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BM3)</f>
         <v>0</v>
       </c>
       <c r="BL2" s="11" cm="1">
-        <f t="array" ref="BL2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BN3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BN4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BN5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BN6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BN7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BN8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BN9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BN10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BN11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BN12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BN13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BN14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BN15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BN16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BN17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BN18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BN19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BN20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BN21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BN22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BN23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BN24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BN25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BN26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BN27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BN28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BN29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BN30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BN31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BN32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BN33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BN3)</f>
+        <f t="array" ref="BL2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BN3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BN4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BN5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BN6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BN7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BN8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BN9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BN10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BN11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BN12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BN13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BN14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BN15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BN16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BN17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BN18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BN19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BN20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BN21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BN22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BN23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BN24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BN25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BN26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BN27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BN28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BN29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BN30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BN31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BN32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BN33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BN3)</f>
         <v>1</v>
       </c>
       <c r="BM2" s="11" cm="1">
-        <f t="array" ref="BM2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BO3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BO4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BO5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BO6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BO7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BO8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BO9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BO10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BO11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BO12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BO13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BO14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BO15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BO16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BO17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BO18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BO19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BO20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BO21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BO22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BO23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BO24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BO25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BO26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BO27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BO28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BO29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BO30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BO31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BO32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BO33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BO3)</f>
+        <f t="array" ref="BM2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BO3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BO4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BO5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BO6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BO7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BO8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BO9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BO10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BO11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BO12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BO13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BO14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BO15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BO16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BO17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BO18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BO19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BO20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BO21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BO22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BO23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BO24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BO25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BO26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BO27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BO28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BO29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BO30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BO31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BO32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BO33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BO3)</f>
         <v>1</v>
       </c>
       <c r="BN2" s="11" cm="1">
-        <f t="array" ref="BN2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BP3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BP4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BP5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BP6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BP7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BP8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BP9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BP10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BP11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BP12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BP13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BP14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BP15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BP16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BP17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BP18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BP19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BP20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BP21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BP22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BP23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BP24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BP25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BP26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BP27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BP28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BP29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BP30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BP31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BP32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BP33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BP3)</f>
+        <f t="array" ref="BN2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BP3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BP4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BP5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BP6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BP7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BP8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BP9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BP10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BP11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BP12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BP13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BP14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BP15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BP16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BP17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BP18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BP19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BP20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BP21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BP22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BP23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BP24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BP25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BP26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BP27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BP28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BP29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BP30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BP31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BP32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BP33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BP3)</f>
         <v>1</v>
       </c>
       <c r="BO2" s="11" cm="1">
-        <f t="array" ref="BO2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BQ3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BQ4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BQ5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BQ6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BQ7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BQ8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BQ9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BQ10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BQ11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BQ12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BQ13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BQ14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BQ15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BQ16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BQ17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BQ18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BQ19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BQ20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BQ21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BQ22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BQ23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BQ24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BQ25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BQ26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BQ27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BQ28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BQ29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BQ30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BQ31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BQ32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BQ33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BQ3)</f>
+        <f t="array" ref="BO2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BQ3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BQ4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BQ5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BQ6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BQ7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BQ8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BQ9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BQ10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BQ11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BQ12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BQ13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BQ14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BQ15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BQ16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BQ17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BQ18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BQ19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BQ20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BQ21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BQ22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BQ23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BQ24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BQ25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BQ26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BQ27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BQ28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BQ29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BQ30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BQ31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BQ32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BQ33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BQ3)</f>
         <v>1</v>
       </c>
       <c r="BP2" s="11" cm="1">
-        <f t="array" ref="BP2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BR3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BR4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BR5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BR6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BR7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BR8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BR9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BR10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BR11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BR12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BR13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BR14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BR15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BR16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BR17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BR18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BR19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BR20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BR21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BR22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BR23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BR24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BR25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BR26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BR27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BR28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BR29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BR30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BR31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BR32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BR33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BR3)</f>
+        <f t="array" ref="BP2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BR3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BR4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BR5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BR6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BR7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BR8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BR9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BR10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BR11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BR12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BR13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BR14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BR15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BR16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BR17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BR18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BR19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BR20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BR21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BR22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BR23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BR24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BR25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BR26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BR27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BR28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BR29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BR30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BR31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BR32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BR33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BR3)</f>
         <v>1</v>
       </c>
       <c r="BQ2" s="11" cm="1">
-        <f t="array" ref="BQ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BS3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BS4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BS5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BS6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BS7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BS8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BS9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BS10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BS11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BS12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BS13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BS14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BS15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BS16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BS17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BS18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BS19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BS20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BS21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BS22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BS23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BS24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BS25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BS26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BS27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BS28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BS29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BS30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BS31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BS32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BS33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BS3)</f>
+        <f t="array" ref="BQ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BS3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BS4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BS5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BS6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BS7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BS8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BS9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BS10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BS11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BS12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BS13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BS14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BS15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BS16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BS17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BS18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BS19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BS20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BS21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BS22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BS23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BS24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BS25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BS26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BS27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BS28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BS29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BS30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BS31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BS32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BS33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BS3)</f>
         <v>1</v>
       </c>
       <c r="BR2" s="11" cm="1">
-        <f t="array" ref="BR2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BT3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BT4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BT5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BT6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BT7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BT8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BT9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BT10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BT11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BT12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BT13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BT14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BT15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BT16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BT17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BT18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BT19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BT20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BT21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BT22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BT23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BT24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BT25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BT26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BT27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BT28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BT29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BT30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BT31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BT32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BT33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BT3)</f>
+        <f t="array" ref="BR2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BT3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BT4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BT5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BT6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BT7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BT8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BT9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BT10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BT11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BT12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BT13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BT14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BT15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BT16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BT17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BT18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BT19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BT20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BT21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BT22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BT23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BT24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BT25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BT26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BT27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BT28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BT29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BT30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BT31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BT32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BT33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BT3)</f>
         <v>0</v>
       </c>
       <c r="BS2" s="11" cm="1">
-        <f t="array" ref="BS2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BU3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BU4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BU5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BU6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BU7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BU8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BU9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BU10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BU11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BU12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BU13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BU14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BU15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BU16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BU17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BU18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BU19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BU20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BU21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BU22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BU23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BU24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BU25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BU26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BU27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BU28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BU29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BU30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BU31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BU32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BU33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BU3)</f>
+        <f t="array" ref="BS2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BU3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BU4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BU5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BU6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BU7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BU8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BU9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BU10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BU11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BU12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BU13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BU14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BU15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BU16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BU17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BU18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BU19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BU20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BU21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BU22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BU23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BU24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BU25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BU26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BU27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BU28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BU29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BU30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BU31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BU32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BU33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BU3)</f>
         <v>0</v>
       </c>
       <c r="BT2" s="11" cm="1">
-        <f t="array" ref="BT2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BV3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BV4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BV5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BV6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BV7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BV8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BV9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BV10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BV11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BV12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BV13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BV14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BV15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BV16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BV17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BV18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BV19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BV20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BV21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BV22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BV23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BV24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BV25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BV26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BV27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BV28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BV29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BV30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BV31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BV32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BV33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BV3)</f>
+        <f t="array" ref="BT2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BV3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BV4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BV5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BV6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BV7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BV8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BV9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BV10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BV11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BV12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BV13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BV14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BV15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BV16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BV17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BV18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BV19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BV20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BV21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BV22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BV23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BV24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BV25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BV26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BV27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BV28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BV29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BV30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BV31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BV32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BV33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BV3)</f>
         <v>0</v>
       </c>
       <c r="BU2" s="11" cm="1">
-        <f t="array" ref="BU2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BW3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BW4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BW5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BW6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BW7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BW8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BW9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BW10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BW11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BW12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BW13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BW14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BW15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BW16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BW17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BW18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BW19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BW20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BW21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BW22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BW23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BW24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BW25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BW26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BW27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BW28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BW29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BW30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BW31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BW32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BW33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BW3)</f>
+        <f t="array" ref="BU2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BW3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BW4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BW5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BW6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BW7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BW8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BW9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BW10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BW11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BW12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BW13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BW14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BW15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BW16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BW17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BW18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BW19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BW20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BW21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BW22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BW23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BW24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BW25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BW26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BW27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BW28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BW29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BW30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BW31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BW32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BW33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BW3)</f>
         <v>1</v>
       </c>
       <c r="BV2" s="11" cm="1">
-        <f t="array" ref="BV2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BX3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BX4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BX5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BX6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BX7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BX8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BX9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BX10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BX11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BX12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BX13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BX14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BX15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BX16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BX17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BX18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BX19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BX20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BX21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BX22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BX23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BX24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BX25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BX26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BX27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BX28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BX29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BX30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BX31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BX32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BX33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BX3)</f>
+        <f t="array" ref="BV2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BX3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BX4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BX5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BX6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BX7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BX8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BX9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BX10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BX11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BX12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BX13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BX14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BX15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BX16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BX17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BX18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BX19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BX20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BX21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BX22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BX23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BX24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BX25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BX26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BX27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BX28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BX29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BX30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BX31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BX32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BX33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BX3)</f>
         <v>1</v>
       </c>
       <c r="BW2" s="11" cm="1">
-        <f t="array" ref="BW2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BY3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BY4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BY5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BY6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BY7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BY8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BY9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BY10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BY11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BY12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BY13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BY14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BY15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BY16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BY17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BY18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BY19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BY20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BY21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BY22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BY23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BY24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BY25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BY26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BY27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BY28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BY29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BY30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BY31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BY32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BY33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BY3)</f>
+        <f t="array" ref="BW2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BY3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BY4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BY5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BY6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BY7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BY8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BY9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BY10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BY11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BY12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BY13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BY14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BY15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BY16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BY17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BY18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BY19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BY20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BY21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BY22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BY23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BY24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BY25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BY26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BY27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BY28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BY29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BY30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BY31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BY32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BY33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BY3)</f>
         <v>1</v>
       </c>
       <c r="BX2" s="11" cm="1">
-        <f t="array" ref="BX2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!BZ3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!BZ4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!BZ5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!BZ6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!BZ7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!BZ8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!BZ9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!BZ10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!BZ11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!BZ12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!BZ13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!BZ14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!BZ15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!BZ16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!BZ17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!BZ18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!BZ19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!BZ20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!BZ21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!BZ22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!BZ23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!BZ24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!BZ25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!BZ26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!BZ27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!BZ28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!BZ29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!BZ30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!BZ31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!BZ32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!BZ33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!BZ3)</f>
+        <f t="array" ref="BX2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!BZ3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!BZ4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!BZ5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!BZ6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!BZ7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!BZ8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!BZ9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!BZ10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!BZ11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!BZ12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!BZ13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!BZ14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!BZ15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!BZ16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!BZ17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!BZ18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!BZ19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!BZ20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!BZ21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!BZ22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!BZ23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!BZ24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!BZ25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!BZ26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!BZ27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!BZ28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!BZ29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!BZ30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!BZ31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!BZ32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!BZ33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!BZ3)</f>
         <v>1</v>
       </c>
       <c r="BY2" s="11" cm="1">
-        <f t="array" ref="BY2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CA3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CA4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CA5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CA6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CA7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CA8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CA9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CA10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CA11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CA12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CA13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CA14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CA15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CA16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CA17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CA18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CA19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CA20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CA21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CA22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CA23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CA24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CA25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CA26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CA27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CA28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CA29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CA30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CA31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CA32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CA33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CA3)</f>
+        <f t="array" ref="BY2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CA3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CA4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CA5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CA6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CA7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CA8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CA9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CA10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CA11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CA12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CA13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CA14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CA15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CA16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CA17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CA18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CA19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CA20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CA21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CA22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CA23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CA24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CA25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CA26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CA27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CA28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CA29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CA30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CA31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CA32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CA33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CA3)</f>
         <v>1</v>
       </c>
       <c r="BZ2" s="11" cm="1">
-        <f t="array" ref="BZ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CB3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CB4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CB5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CB6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CB7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CB8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CB9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CB10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CB11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CB12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CB13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CB14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CB15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CB16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CB17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CB18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CB19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CB20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CB21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CB22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CB23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CB24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CB25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CB26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CB27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CB28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CB29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CB30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CB31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CB32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CB33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CB3)</f>
+        <f t="array" ref="BZ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CB3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CB4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CB5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CB6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CB7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CB8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CB9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CB10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CB11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CB12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CB13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CB14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CB15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CB16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CB17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CB18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CB19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CB20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CB21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CB22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CB23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CB24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CB25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CB26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CB27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CB28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CB29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CB30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CB31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CB32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CB33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CB3)</f>
         <v>1</v>
       </c>
       <c r="CA2" s="11" cm="1">
-        <f t="array" ref="CA2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CC3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CC4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CC5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CC6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CC7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CC8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CC9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CC10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CC11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CC12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CC13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CC14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CC15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CC16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CC17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CC18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CC19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CC20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CC21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CC22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CC23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CC24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CC25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CC26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CC27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CC28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CC29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CC30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CC31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CC32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CC33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CC3)</f>
+        <f t="array" ref="CA2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CC3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CC4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CC5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CC6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CC7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CC8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CC9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CC10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CC11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CC12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CC13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CC14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CC15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CC16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CC17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CC18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CC19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CC20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CC21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CC22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CC23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CC24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CC25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CC26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CC27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CC28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CC29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CC30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CC31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CC32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CC33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CC3)</f>
         <v>0</v>
       </c>
       <c r="CB2" s="11" cm="1">
-        <f t="array" ref="CB2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CD3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CD4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CD5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CD6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CD7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CD8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CD9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CD10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CD11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CD12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CD13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CD14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CD15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CD16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CD17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CD18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CD19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CD20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CD21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CD22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CD23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CD24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CD25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CD26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CD27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CD28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CD29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CD30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CD31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CD32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CD33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CD3)</f>
+        <f t="array" ref="CB2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CD3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CD4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CD5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CD6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CD7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CD8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CD9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CD10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CD11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CD12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CD13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CD14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CD15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CD16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CD17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CD18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CD19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CD20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CD21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CD22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CD23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CD24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CD25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CD26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CD27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CD28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CD29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CD30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CD31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CD32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CD33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CD3)</f>
         <v>0</v>
       </c>
       <c r="CC2" s="11" cm="1">
-        <f t="array" ref="CC2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CE3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CE4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CE5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CE6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CE7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CE8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CE9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CE10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CE11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CE12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CE13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CE14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CE15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CE16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CE17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CE18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CE19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CE20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CE21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CE22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CE23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CE24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CE25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CE26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CE27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CE28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CE29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CE30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CE31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CE32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CE33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CE3)</f>
+        <f t="array" ref="CC2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CE3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CE4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CE5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CE6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CE7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CE8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CE9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CE10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CE11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CE12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CE13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CE14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CE15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CE16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CE17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CE18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CE19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CE20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CE21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CE22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CE23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CE24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CE25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CE26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CE27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CE28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CE29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CE30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CE31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CE32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CE33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CE3)</f>
         <v>0</v>
       </c>
       <c r="CD2" s="11" cm="1">
-        <f t="array" ref="CD2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CF3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CF4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CF5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CF6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CF7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CF8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CF9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CF10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CF11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CF12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CF13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CF14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CF15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CF16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CF17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CF18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CF19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CF20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CF21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CF22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CF23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CF24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CF25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CF26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CF27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CF28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CF29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CF30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CF31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CF32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CF33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CF3)</f>
+        <f t="array" ref="CD2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CF3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CF4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CF5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CF6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CF7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CF8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CF9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CF10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CF11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CF12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CF13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CF14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CF15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CF16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CF17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CF18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CF19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CF20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CF21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CF22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CF23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CF24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CF25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CF26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CF27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CF28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CF29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CF30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CF31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CF32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CF33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CF3)</f>
         <v>1</v>
       </c>
       <c r="CE2" s="11" cm="1">
-        <f t="array" ref="CE2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CG3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CG4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CG5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CG6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CG7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CG8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CG9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CG10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CG11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CG12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CG13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CG14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CG15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CG16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CG17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CG18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CG19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CG20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CG21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CG22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CG23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CG24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CG25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CG26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CG27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CG28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CG29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CG30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CG31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CG32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CG33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CG3)</f>
+        <f t="array" ref="CE2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CG3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CG4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CG5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CG6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CG7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CG8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CG9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CG10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CG11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CG12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CG13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CG14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CG15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CG16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CG17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CG18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CG19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CG20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CG21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CG22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CG23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CG24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CG25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CG26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CG27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CG28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CG29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CG30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CG31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CG32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CG33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CG3)</f>
         <v>1</v>
       </c>
       <c r="CF2" s="11" cm="1">
-        <f t="array" ref="CF2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CH3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CH4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CH5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CH6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CH7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CH8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CH9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CH10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CH11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CH12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CH13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CH14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CH15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CH16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CH17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CH18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CH19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CH20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CH21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CH22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CH23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CH24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CH25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CH26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CH27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CH28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CH29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CH30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CH31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CH32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CH33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CH3)</f>
+        <f t="array" ref="CF2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CH3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CH4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CH5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CH6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CH7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CH8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CH9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CH10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CH11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CH12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CH13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CH14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CH15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CH16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CH17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CH18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CH19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CH20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CH21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CH22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CH23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CH24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CH25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CH26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CH27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CH28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CH29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CH30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CH31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CH32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CH33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CH3)</f>
         <v>1</v>
       </c>
       <c r="CG2" s="11" cm="1">
-        <f t="array" ref="CG2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CI3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CI4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CI5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CI6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CI7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CI8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CI9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CI10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CI11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CI12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CI13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CI14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CI15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CI16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CI17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CI18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CI19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CI20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CI21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CI22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CI23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CI24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CI25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CI26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CI27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CI28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CI29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CI30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CI31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CI32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CI33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CI3)</f>
+        <f t="array" ref="CG2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CI3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CI4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CI5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CI6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CI7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CI8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CI9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CI10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CI11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CI12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CI13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CI14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CI15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CI16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CI17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CI18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CI19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CI20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CI21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CI22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CI23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CI24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CI25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CI26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CI27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CI28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CI29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CI30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CI31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CI32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CI33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CI3)</f>
         <v>1</v>
       </c>
       <c r="CH2" s="11" cm="1">
-        <f t="array" ref="CH2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CJ3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CJ4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CJ5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CJ6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CJ7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CJ8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CJ9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CJ10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CJ11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CJ12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CJ13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CJ14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CJ15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CJ16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CJ17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CJ18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CJ19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CJ20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CJ21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CJ22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CJ23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CJ24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CJ25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CJ26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CJ27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CJ28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CJ29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CJ30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CJ31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CJ32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CJ33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CJ3)</f>
+        <f t="array" ref="CH2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CJ3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CJ4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CJ5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CJ6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CJ7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CJ8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CJ9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CJ10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CJ11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CJ12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CJ13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CJ14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CJ15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CJ16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CJ17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CJ18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CJ19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CJ20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CJ21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CJ22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CJ23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CJ24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CJ25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CJ26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CJ27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CJ28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CJ29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CJ30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CJ31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CJ32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CJ33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CJ3)</f>
         <v>1</v>
       </c>
       <c r="CI2" s="11" cm="1">
-        <f t="array" ref="CI2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CK3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CK4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CK5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CK6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CK7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CK8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CK9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CK10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CK11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CK12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CK13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CK14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CK15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CK16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CK17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CK18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CK19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CK20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CK21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CK22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CK23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CK24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CK25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CK26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CK27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CK28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CK29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CK30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CK31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CK32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CK33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CK3)</f>
+        <f t="array" ref="CI2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CK3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CK4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CK5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CK6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CK7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CK8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CK9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CK10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CK11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CK12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CK13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CK14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CK15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CK16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CK17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CK18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CK19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CK20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CK21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CK22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CK23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CK24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CK25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CK26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CK27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CK28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CK29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CK30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CK31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CK32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CK33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CK3)</f>
         <v>1</v>
       </c>
       <c r="CJ2" s="11" cm="1">
-        <f t="array" ref="CJ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CL3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CL4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CL5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CL6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CL7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CL8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CL9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CL10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CL11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CL12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CL13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CL14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CL15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CL16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CL17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CL18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CL19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CL20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CL21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CL22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CL23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CL24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CL25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CL26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CL27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CL28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CL29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CL30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CL31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CL32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CL33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CL3)</f>
+        <f t="array" ref="CJ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CL3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CL4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CL5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CL6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CL7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CL8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CL9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CL10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CL11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CL12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CL13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CL14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CL15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CL16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CL17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CL18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CL19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CL20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CL21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CL22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CL23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CL24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CL25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CL26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CL27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CL28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CL29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CL30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CL31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CL32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CL33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CL3)</f>
         <v>0</v>
       </c>
       <c r="CK2" s="11" cm="1">
-        <f t="array" ref="CK2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CM3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CM4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CM5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CM6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CM7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CM8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CM9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CM10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CM11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CM12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CM13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CM14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CM15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CM16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CM17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CM18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CM19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CM20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CM21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CM22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CM23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CM24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CM25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CM26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CM27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CM28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CM29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CM30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CM31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CM32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CM33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CM3)</f>
+        <f t="array" ref="CK2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CM3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CM4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CM5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CM6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CM7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CM8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CM9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CM10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CM11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CM12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CM13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CM14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CM15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CM16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CM17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CM18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CM19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CM20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CM21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CM22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CM23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CM24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CM25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CM26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CM27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CM28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CM29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CM30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CM31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CM32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CM33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CM3)</f>
         <v>0</v>
       </c>
       <c r="CL2" s="11" cm="1">
-        <f t="array" ref="CL2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CN3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CN4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CN5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CN6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CN7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CN8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CN9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CN10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CN11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CN12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CN13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CN14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CN15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CN16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CN17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CN18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CN19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CN20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CN21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CN22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CN23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CN24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CN25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CN26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CN27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CN28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CN29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CN30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CN31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CN32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CN33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CN3)</f>
+        <f t="array" ref="CL2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CN3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CN4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CN5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CN6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CN7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CN8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CN9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CN10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CN11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CN12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CN13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CN14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CN15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CN16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CN17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CN18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CN19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CN20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CN21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CN22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CN23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CN24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CN25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CN26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CN27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CN28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CN29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CN30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CN31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CN32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CN33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CN3)</f>
         <v>0</v>
       </c>
       <c r="CM2" s="11" cm="1">
-        <f t="array" ref="CM2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CO3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CO4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CO5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CO6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CO7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CO8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CO9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CO10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CO11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CO12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CO13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CO14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CO15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CO16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CO17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CO18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CO19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CO20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CO21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CO22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CO23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CO24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CO25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CO26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CO27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CO28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CO29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CO30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CO31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CO32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CO33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CO3)</f>
+        <f t="array" ref="CM2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CO3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CO4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CO5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CO6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CO7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CO8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CO9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CO10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CO11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CO12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CO13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CO14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CO15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CO16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CO17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CO18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CO19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CO20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CO21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CO22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CO23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CO24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CO25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CO26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CO27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CO28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CO29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CO30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CO31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CO32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CO33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CO3)</f>
         <v>1</v>
       </c>
       <c r="CN2" s="11" cm="1">
-        <f t="array" ref="CN2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CP3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CP4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CP5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CP6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CP7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CP8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CP9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CP10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CP11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CP12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CP13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CP14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CP15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CP16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CP17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CP18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CP19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CP20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CP21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CP22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CP23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CP24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CP25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CP26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CP27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CP28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CP29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CP30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CP31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CP32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CP33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CP3)</f>
+        <f t="array" ref="CN2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CP3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CP4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CP5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CP6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CP7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CP8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CP9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CP10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CP11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CP12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CP13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CP14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CP15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CP16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CP17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CP18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CP19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CP20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CP21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CP22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CP23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CP24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CP25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CP26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CP27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CP28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CP29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CP30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CP31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CP32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CP33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CP3)</f>
         <v>1</v>
       </c>
       <c r="CO2" s="11" cm="1">
-        <f t="array" ref="CO2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CQ3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CQ4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CQ5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CQ6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CQ7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CQ8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CQ9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CQ10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CQ11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CQ12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CQ13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CQ14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CQ15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CQ16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CQ17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CQ18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CQ19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CQ20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CQ21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CQ22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CQ23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CQ24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CQ25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CQ26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CQ27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CQ28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CQ29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CQ30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CQ31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CQ32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CQ33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CQ3)</f>
+        <f t="array" ref="CO2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CQ3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CQ4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CQ5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CQ6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CQ7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CQ8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CQ9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CQ10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CQ11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CQ12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CQ13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CQ14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CQ15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CQ16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CQ17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CQ18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CQ19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CQ20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CQ21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CQ22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CQ23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CQ24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CQ25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CQ26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CQ27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CQ28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CQ29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CQ30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CQ31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CQ32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CQ33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CQ3)</f>
         <v>1</v>
       </c>
       <c r="CP2" s="11" cm="1">
-        <f t="array" ref="CP2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CR3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CR4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CR5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CR6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CR7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CR8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CR9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CR10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CR11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CR12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CR13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CR14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CR15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CR16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CR17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CR18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CR19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CR20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CR21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CR22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CR23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CR24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CR25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CR26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CR27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CR28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CR29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CR30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CR31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CR32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CR33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CR3)</f>
+        <f t="array" ref="CP2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CR3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CR4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CR5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CR6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CR7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CR8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CR9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CR10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CR11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CR12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CR13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CR14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CR15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CR16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CR17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CR18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CR19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CR20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CR21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CR22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CR23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CR24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CR25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CR26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CR27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CR28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CR29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CR30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CR31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CR32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CR33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CR3)</f>
         <v>1</v>
       </c>
       <c r="CQ2" s="11" cm="1">
-        <f t="array" ref="CQ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CS3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CS4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CS5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CS6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CS7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CS8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CS9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CS10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CS11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CS12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CS13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CS14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CS15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CS16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CS17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CS18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CS19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CS20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CS21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CS22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CS23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CS24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CS25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CS26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CS27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CS28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CS29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CS30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CS31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CS32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CS33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CS3)</f>
+        <f t="array" ref="CQ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CS3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CS4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CS5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CS6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CS7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CS8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CS9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CS10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CS11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CS12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CS13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CS14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CS15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CS16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CS17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CS18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CS19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CS20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CS21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CS22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CS23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CS24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CS25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CS26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CS27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CS28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CS29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CS30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CS31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CS32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CS33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CS3)</f>
         <v>1</v>
       </c>
       <c r="CR2" s="11" cm="1">
-        <f t="array" ref="CR2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CT3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CT4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CT5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CT6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CT7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CT8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CT9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CT10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CT11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CT12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CT13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CT14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CT15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CT16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CT17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CT18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CT19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CT20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CT21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CT22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CT23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CT24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CT25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CT26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CT27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CT28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CT29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CT30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CT31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CT32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CT33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CT3)</f>
+        <f t="array" ref="CR2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CT3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CT4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CT5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CT6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CT7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CT8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CT9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CT10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CT11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CT12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CT13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CT14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CT15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CT16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CT17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CT18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CT19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CT20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CT21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CT22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CT23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CT24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CT25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CT26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CT27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CT28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CT29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CT30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CT31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CT32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CT33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CT3)</f>
         <v>1</v>
       </c>
       <c r="CS2" s="11" cm="1">
-        <f t="array" ref="CS2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CU3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CU4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CU5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CU6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CU7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CU8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CU9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CU10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CU11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CU12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CU13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CU14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CU15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CU16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CU17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CU18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CU19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CU20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CU21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CU22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CU23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CU24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CU25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CU26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CU27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CU28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CU29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CU30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CU31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CU32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CU33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CU3)</f>
+        <f t="array" ref="CS2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CU3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CU4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CU5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CU6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CU7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CU8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CU9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CU10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CU11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CU12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CU13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CU14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CU15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CU16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CU17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CU18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CU19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CU20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CU21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CU22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CU23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CU24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CU25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CU26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CU27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CU28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CU29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CU30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CU31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CU32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CU33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CU3)</f>
         <v>0</v>
       </c>
       <c r="CT2" s="11" cm="1">
-        <f t="array" ref="CT2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CV3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CV4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CV5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CV6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CV7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CV8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CV9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CV10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CV11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CV12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CV13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CV14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CV15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CV16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CV17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CV18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CV19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CV20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CV21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CV22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CV23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CV24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CV25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CV26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CV27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CV28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CV29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CV30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CV31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CV32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CV33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CV3)</f>
+        <f t="array" ref="CT2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CV3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CV4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CV5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CV6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CV7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CV8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CV9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CV10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CV11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CV12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CV13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CV14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CV15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CV16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CV17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CV18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CV19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CV20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CV21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CV22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CV23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CV24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CV25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CV26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CV27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CV28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CV29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CV30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CV31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CV32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CV33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CV3)</f>
         <v>0</v>
       </c>
       <c r="CU2" s="11" cm="1">
-        <f t="array" ref="CU2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CW3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CW4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CW5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CW6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CW7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CW8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CW9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CW10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CW11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CW12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CW13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CW14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CW15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CW16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CW17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CW18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CW19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CW20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CW21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CW22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CW23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CW24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CW25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CW26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CW27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CW28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CW29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CW30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CW31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CW32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CW33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CW3)</f>
+        <f t="array" ref="CU2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CW3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CW4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CW5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CW6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CW7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CW8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CW9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CW10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CW11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CW12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CW13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CW14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CW15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CW16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CW17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CW18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CW19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CW20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CW21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CW22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CW23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CW24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CW25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CW26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CW27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CW28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CW29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CW30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CW31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CW32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CW33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CW3)</f>
         <v>0</v>
       </c>
       <c r="CV2" s="11" cm="1">
-        <f t="array" ref="CV2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CX3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CX4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CX5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CX6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CX7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CX8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CX9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CX10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CX11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CX12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CX13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CX14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CX15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CX16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CX17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CX18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CX19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CX20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CX21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CX22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CX23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CX24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CX25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CX26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CX27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CX28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CX29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CX30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CX31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CX32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CX33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CX3)</f>
+        <f t="array" ref="CV2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CX3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CX4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CX5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CX6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CX7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CX8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CX9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CX10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CX11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CX12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CX13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CX14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CX15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CX16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CX17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CX18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CX19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CX20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CX21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CX22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CX23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CX24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CX25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CX26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CX27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CX28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CX29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CX30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CX31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CX32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CX33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CX3)</f>
         <v>1</v>
       </c>
       <c r="CW2" s="11" cm="1">
-        <f t="array" ref="CW2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CY3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CY4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CY5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CY6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CY7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CY8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CY9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CY10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CY11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CY12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CY13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CY14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CY15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CY16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CY17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CY18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CY19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CY20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CY21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CY22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CY23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CY24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CY25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CY26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CY27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CY28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CY29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CY30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CY31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CY32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CY33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CY3)</f>
+        <f t="array" ref="CW2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CY3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CY4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CY5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CY6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CY7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CY8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CY9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CY10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CY11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CY12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CY13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CY14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CY15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CY16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CY17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CY18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CY19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CY20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CY21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CY22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CY23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CY24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CY25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CY26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CY27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CY28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CY29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CY30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CY31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CY32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CY33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CY3)</f>
         <v>1</v>
       </c>
       <c r="CX2" s="11" cm="1">
-        <f t="array" ref="CX2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!CZ3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!CZ4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!CZ5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!CZ6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!CZ7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!CZ8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!CZ9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!CZ10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!CZ11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!CZ12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!CZ13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!CZ14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!CZ15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!CZ16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!CZ17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!CZ18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!CZ19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!CZ20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!CZ21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!CZ22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!CZ23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!CZ24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!CZ25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!CZ26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!CZ27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!CZ28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!CZ29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!CZ30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!CZ31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!CZ32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!CZ33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!CZ3)</f>
+        <f t="array" ref="CX2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!CZ3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!CZ4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!CZ5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!CZ6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!CZ7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!CZ8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!CZ9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!CZ10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!CZ11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!CZ12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!CZ13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!CZ14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!CZ15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!CZ16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!CZ17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!CZ18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!CZ19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!CZ20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!CZ21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!CZ22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!CZ23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!CZ24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!CZ25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!CZ26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!CZ27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!CZ28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!CZ29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!CZ30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!CZ31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!CZ32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!CZ33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!CZ3)</f>
         <v>1</v>
       </c>
       <c r="CY2" s="11" cm="1">
-        <f t="array" ref="CY2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!DA3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!DA4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!DA5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!DA6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!DA7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!DA8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!DA9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!DA10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!DA11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!DA12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!DA13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!DA14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!DA15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!DA16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!DA17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!DA18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!DA19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!DA20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!DA21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!DA22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!DA23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!DA24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!DA25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!DA26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!DA27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!DA28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!DA29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!DA30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!DA31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!DA32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!DA33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!DA3)</f>
+        <f t="array" ref="CY2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!DA3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!DA4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!DA5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!DA6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!DA7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!DA8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!DA9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!DA10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!DA11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!DA12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!DA13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!DA14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!DA15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!DA16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!DA17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!DA18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!DA19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!DA20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!DA21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!DA22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!DA23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!DA24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!DA25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!DA26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!DA27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!DA28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!DA29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!DA30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!DA31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!DA32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!DA33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!DA3)</f>
         <v>1</v>
       </c>
       <c r="CZ2" s="11" cm="1">
-        <f t="array" ref="CZ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!DB3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!DB4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!DB5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!DB6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!DB7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!DB8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!DB9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!DB10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!DB11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!DB12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!DB13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!DB14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!DB15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!DB16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!DB17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!DB18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!DB19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!DB20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!DB21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!DB22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!DB23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!DB24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!DB25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!DB26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!DB27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!DB28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!DB29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!DB30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!DB31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!DB32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!DB33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!DB3)</f>
+        <f t="array" ref="CZ2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!DB3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!DB4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!DB5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!DB6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!DB7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!DB8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!DB9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!DB10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!DB11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!DB12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!DB13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!DB14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!DB15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!DB16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!DB17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!DB18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!DB19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!DB20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!DB21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!DB22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!DB23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!DB24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!DB25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!DB26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!DB27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!DB28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!DB29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!DB30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!DB31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!DB32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!DB33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!DB3)</f>
         <v>1</v>
       </c>
       <c r="DA2" s="11" cm="1">
-        <f t="array" ref="DA2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!DC3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!DC4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!DC5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!DC6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!DC7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!DC8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!DC9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!DC10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!DC11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!DC12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!DC13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!DC14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!DC15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!DC16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!DC17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!DC18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!DC19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!DC20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!DC21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!DC22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!DC23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!DC24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!DC25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!DC26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!DC27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!DC28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!DC29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!DC30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!DC31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!DC32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!DC33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!DC3)</f>
+        <f t="array" ref="DA2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!DC3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!DC4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!DC5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!DC6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!DC7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!DC8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!DC9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!DC10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!DC11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!DC12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!DC13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!DC14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!DC15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!DC16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!DC17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!DC18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!DC19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!DC20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!DC21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!DC22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!DC23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!DC24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!DC25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!DC26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!DC27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!DC28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!DC29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!DC30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!DC31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!DC32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!DC33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!DC3)</f>
         <v>1</v>
       </c>
       <c r="DB2" s="11" cm="1">
-        <f t="array" ref="DB2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!DD3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!DD4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!DD5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!DD6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!DD7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!DD8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!DD9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!DD10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!DD11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!DD12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!DD13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!DD14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!DD15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!DD16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!DD17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!DD18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!DD19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!DD20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!DD21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!DD22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!DD23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!DD24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!DD25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!DD26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!DD27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!DD28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!DD29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!DD30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!DD31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!DD32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!DD33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!DD3)</f>
+        <f t="array" ref="DB2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!DD3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!DD4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!DD5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!DD6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!DD7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!DD8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!DD9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!DD10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!DD11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!DD12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!DD13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!DD14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!DD15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!DD16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!DD17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!DD18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!DD19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!DD20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!DD21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!DD22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!DD23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!DD24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!DD25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!DD26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!DD27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!DD28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!DD29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!DD30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!DD31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!DD32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!DD33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!DD3)</f>
         <v>0</v>
       </c>
       <c r="DC2" s="11" cm="1">
-        <f t="array" ref="DC2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!DE3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!DE4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!DE5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!DE6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!DE7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!DE8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!DE9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!DE10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!DE11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!DE12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!DE13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!DE14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!DE15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!DE16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!DE17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!DE18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!DE19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!DE20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!DE21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!DE22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!DE23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!DE24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!DE25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!DE26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!DE27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!DE28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!DE29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!DE30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!DE31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!DE32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!DE33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!DE3)</f>
+        <f t="array" ref="DC2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!DE3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!DE4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!DE5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!DE6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!DE7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!DE8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!DE9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!DE10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!DE11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!DE12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!DE13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!DE14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!DE15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!DE16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!DE17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!DE18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!DE19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!DE20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!DE21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!DE22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!DE23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!DE24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!DE25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!DE26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!DE27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!DE28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!DE29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!DE30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!DE31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!DE32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!DE33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!DE3)</f>
         <v>0</v>
       </c>
       <c r="DD2" s="11" cm="1">
-        <f t="array" ref="DD2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های عمومی'!A3,'شاخص‌های عمومی'!DF3,'شاخص‌های عمومی'!A4,'شاخص‌های عمومی'!DF4,'شاخص‌های عمومی'!A5,'شاخص‌های عمومی'!DF5,'شاخص‌های عمومی'!A6,'شاخص‌های عمومی'!DF6,'شاخص‌های عمومی'!A7,'شاخص‌های عمومی'!DF7,'شاخص‌های عمومی'!A8,'شاخص‌های عمومی'!DF8,'شاخص‌های عمومی'!A9,'شاخص‌های عمومی'!DF9,'شاخص‌های عمومی'!A10,'شاخص‌های عمومی'!DF10,'شاخص‌های عمومی'!A11,'شاخص‌های عمومی'!DF11,'شاخص‌های عمومی'!A12,'شاخص‌های عمومی'!DF12,'شاخص‌های عمومی'!A13,'شاخص‌های عمومی'!DF13,'شاخص‌های عمومی'!A14,'شاخص‌های عمومی'!DF14,'شاخص‌های عمومی'!A15,'شاخص‌های عمومی'!DF15,'شاخص‌های عمومی'!A16,'شاخص‌های عمومی'!DF16,'شاخص‌های عمومی'!A17,'شاخص‌های عمومی'!DF17,'شاخص‌های عمومی'!A18,'شاخص‌های عمومی'!DF18,'شاخص‌های عمومی'!A19,'شاخص‌های عمومی'!DF19,'شاخص‌های عمومی'!A20,'شاخص‌های عمومی'!DF20,'شاخص‌های عمومی'!A21,'شاخص‌های عمومی'!DF21,'شاخص‌های عمومی'!A22,'شاخص‌های عمومی'!DF22,'شاخص‌های عمومی'!A23,'شاخص‌های عمومی'!DF23,'شاخص‌های عمومی'!A24,'شاخص‌های عمومی'!DF24,'شاخص‌های عمومی'!A25,'شاخص‌های عمومی'!DF25,'شاخص‌های عمومی'!A26,'شاخص‌های عمومی'!DF26,'شاخص‌های عمومی'!A27,'شاخص‌های عمومی'!DF27,'شاخص‌های عمومی'!A28,'شاخص‌های عمومی'!DF28,'شاخص‌های عمومی'!A29,'شاخص‌های عمومی'!DF29,'شاخص‌های عمومی'!A30,'شاخص‌های عمومی'!DF30,'شاخص‌های عمومی'!A31,'شاخص‌های عمومی'!DF31,'شاخص‌های عمومی'!A32,'شاخص‌های عمومی'!DF32,'شاخص‌های عمومی'!A33,'شاخص‌های عمومی'!DF33,'شاخص‌های عمومی'!A34,'شاخص‌های عمومی'!DF3)</f>
+        <f t="array" ref="DD2">_xlfn.SWITCH('صفحه اصلی'!B4,'شاخص‌های مدیریتی و فرماندهی'!A3,'شاخص‌های مدیریتی و فرماندهی'!DF3,'شاخص‌های مدیریتی و فرماندهی'!A4,'شاخص‌های مدیریتی و فرماندهی'!DF4,'شاخص‌های مدیریتی و فرماندهی'!A5,'شاخص‌های مدیریتی و فرماندهی'!DF5,'شاخص‌های مدیریتی و فرماندهی'!A6,'شاخص‌های مدیریتی و فرماندهی'!DF6,'شاخص‌های مدیریتی و فرماندهی'!A7,'شاخص‌های مدیریتی و فرماندهی'!DF7,'شاخص‌های مدیریتی و فرماندهی'!A8,'شاخص‌های مدیریتی و فرماندهی'!DF8,'شاخص‌های مدیریتی و فرماندهی'!A9,'شاخص‌های مدیریتی و فرماندهی'!DF9,'شاخص‌های مدیریتی و فرماندهی'!A10,'شاخص‌های مدیریتی و فرماندهی'!DF10,'شاخص‌های مدیریتی و فرماندهی'!A11,'شاخص‌های مدیریتی و فرماندهی'!DF11,'شاخص‌های مدیریتی و فرماندهی'!A12,'شاخص‌های مدیریتی و فرماندهی'!DF12,'شاخص‌های مدیریتی و فرماندهی'!A13,'شاخص‌های مدیریتی و فرماندهی'!DF13,'شاخص‌های مدیریتی و فرماندهی'!A14,'شاخص‌های مدیریتی و فرماندهی'!DF14,'شاخص‌های مدیریتی و فرماندهی'!A15,'شاخص‌های مدیریتی و فرماندهی'!DF15,'شاخص‌های مدیریتی و فرماندهی'!A16,'شاخص‌های مدیریتی و فرماندهی'!DF16,'شاخص‌های مدیریتی و فرماندهی'!A17,'شاخص‌های مدیریتی و فرماندهی'!DF17,'شاخص‌های مدیریتی و فرماندهی'!A18,'شاخص‌های مدیریتی و فرماندهی'!DF18,'شاخص‌های مدیریتی و فرماندهی'!A19,'شاخص‌های مدیریتی و فرماندهی'!DF19,'شاخص‌های مدیریتی و فرماندهی'!A20,'شاخص‌های مدیریتی و فرماندهی'!DF20,'شاخص‌های مدیریتی و فرماندهی'!A21,'شاخص‌های مدیریتی و فرماندهی'!DF21,'شاخص‌های مدیریتی و فرماندهی'!A22,'شاخص‌های مدیریتی و فرماندهی'!DF22,'شاخص‌های مدیریتی و فرماندهی'!A23,'شاخص‌های مدیریتی و فرماندهی'!DF23,'شاخص‌های مدیریتی و فرماندهی'!A24,'شاخص‌های مدیریتی و فرماندهی'!DF24,'شاخص‌های مدیریتی و فرماندهی'!A25,'شاخص‌های مدیریتی و فرماندهی'!DF25,'شاخص‌های مدیریتی و فرماندهی'!A26,'شاخص‌های مدیریتی و فرماندهی'!DF26,'شاخص‌های مدیریتی و فرماندهی'!A27,'شاخص‌های مدیریتی و فرماندهی'!DF27,'شاخص‌های مدیریتی و فرماندهی'!A28,'شاخص‌های مدیریتی و فرماندهی'!DF28,'شاخص‌های مدیریتی و فرماندهی'!A29,'شاخص‌های مدیریتی و فرماندهی'!DF29,'شاخص‌های مدیریتی و فرماندهی'!A30,'شاخص‌های مدیریتی و فرماندهی'!DF30,'شاخص‌های مدیریتی و فرماندهی'!A31,'شاخص‌های مدیریتی و فرماندهی'!DF31,'شاخص‌های مدیریتی و فرماندهی'!A32,'شاخص‌های مدیریتی و فرماندهی'!DF32,'شاخص‌های مدیریتی و فرماندهی'!A33,'شاخص‌های مدیریتی و فرماندهی'!DF33,'شاخص‌های مدیریتی و فرماندهی'!A34,'شاخص‌های مدیریتی و فرماندهی'!DF3)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>